<commit_message>
dep time update due to rg removal
</commit_message>
<xml_diff>
--- a/Exports/entire_solution.xlsx
+++ b/Exports/entire_solution.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H176"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,27 +477,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.96</v>
+        <v>3.8</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[((1, 3), 0, 0), ((1, 3), 0.2, 0), ((1, 3), 0.4, 0), ((1, 3), 0.6, 0), ((1, 3), 0.8, 0), ((1, 3), 1.0, 0), ((1, 3), 1.2, 0), ((1, 3), 1.4, 0), ((1, 3), 1.6, 0), ((1, 3), 1.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[((1, 2), 0, 0), ((1, 2), 7.96, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 0, 0), ((1, 3), 0.2, 0), ((1, 3), 0.4, 0), ((1, 3), 0.6, 0), ((1, 3), 0.8, 0), ((1, 3), 1.0, 0), ((1, 3), 1.2, 0), ((1, 3), 1.4, 0), ((1, 3), 1.6, 0), ((1, 3), 1.8, 0), ((1, 3), 2.0, 0), ((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>78.55999999999999</v>
+        <v>38</v>
       </c>
       <c r="G2" t="n">
-        <v>131.34</v>
+        <v>238.8</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -507,24 +503,20 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13.93</v>
+        <v>9.77</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[((1, 3), 0, 0), ((1, 3), 0.2, 0), ((1, 3), 0.4, 0), ((1, 3), 0.6, 0), ((1, 3), 0.8, 0), ((1, 3), 1.0, 0), ((1, 3), 1.2, 0), ((1, 3), 1.4, 0), ((1, 3), 1.6, 0), ((1, 3), 1.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>[((2, 3), 0, 0), ((2, 3), 0.2, 0), ((2, 3), 0.4, 0), ((2, 3), 0.6, 0), ((2, 3), 0.8, 0), ((2, 3), 1.0, 0), ((2, 3), 1.2, 0), ((2, 3), 1.4, 0), ((2, 3), 1.6, 0), ((2, 3), 1.8, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 0, 0), ((1, 3), 0.2, 0), ((1, 3), 0.4, 0), ((1, 3), 0.6, 0), ((1, 3), 0.8, 0), ((1, 3), 1.0, 0), ((1, 3), 1.2, 0), ((1, 3), 1.4, 0), ((1, 3), 1.6, 0), ((1, 3), 1.8, 0), ((1, 3), 2.0, 0), ((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>130.3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -537,7 +529,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.9</v>
+        <v>15.74</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -551,10 +543,10 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>63.67999999999999</v>
+        <v>47.04</v>
       </c>
       <c r="G4" t="n">
-        <v>35.82000000000001</v>
+        <v>35.82</v>
       </c>
       <c r="H4" t="n">
         <v>0.2</v>
@@ -567,7 +559,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25.87</v>
+        <v>21.71</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -581,7 +573,7 @@
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>25.87</v>
+        <v>21.71</v>
       </c>
       <c r="G5" t="n">
         <v>5.969999999999999</v>
@@ -597,7 +589,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>31.84</v>
+        <v>27.68</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -619,23 +611,23 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>32.4</v>
+        <v>28.2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.6, 0), ((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0)]</t>
+          <t>[((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0), ((1, 3), 26.2, 0), ((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>8.999999999999982</v>
+        <v>37.99999999999997</v>
       </c>
       <c r="G7" t="n">
-        <v>167.7000000000001</v>
+        <v>238.8</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -645,24 +637,20 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>43.2</v>
+        <v>34.17</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.6, 0), ((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0)]</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>[((2, 3), 41.4, 0), ((2, 3), 41.6, 0), ((2, 3), 41.8, 0), ((2, 3), 42.0, 0), ((2, 3), 42.2, 0), ((2, 3), 42.4, 0), ((2, 3), 42.6, 0), ((2, 3), 42.8, 0), ((2, 3), 43.0, 0), ((2, 3), 43.2, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0), ((1, 3), 26.2, 0), ((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>9.000000000000028</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -675,7 +663,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49.17</v>
+        <v>40.14</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -741,7 +729,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[((1, 3), 6.0, 0), ((1, 3), 6.2, 0), ((1, 3), 6.4, 0), ((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0)]</t>
+          <t>[((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0), ((1, 3), 39.4, 0), ((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0), ((1, 3), 40.6, 0)]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -751,13 +739,13 @@
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>496.16</v>
+        <v>185.28</v>
       </c>
       <c r="G12" t="n">
-        <v>131.34</v>
+        <v>143.28</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="13">
@@ -771,20 +759,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[((1, 3), 6.0, 0), ((1, 3), 6.2, 0), ((1, 3), 6.4, 0), ((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0)]</t>
+          <t>[((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0), ((1, 3), 39.4, 0), ((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0), ((1, 3), 40.6, 0)]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[((2, 3), 6.0, 0), ((2, 3), 6.2, 0), ((2, 3), 6.4, 0), ((2, 3), 6.6, 0), ((2, 3), 6.8, 0), ((2, 3), 7.0, 0), ((2, 3), 7.2, 0), ((2, 3), 7.4, 0), ((2, 3), 7.6, 0), ((2, 3), 7.8, 0)]</t>
+          <t>[((2, 3), 5.4, 0), ((2, 3), 5.6, 0), ((2, 3), 5.8, 0), ((2, 3), 6.0, 0), ((2, 3), 6.2, 0), ((2, 3), 6.4, 0), ((2, 3), 6.6, 0), ((2, 3), 6.8, 0), ((2, 3), 7.0, 0)]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>547.9</v>
+        <v>499.41</v>
       </c>
       <c r="G13" t="n">
-        <v>59.69999999999999</v>
+        <v>53.72999999999999</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -799,25 +787,17 @@
       <c r="B14" t="n">
         <v>67.66</v>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>[((3, 5), 47.76, 0), ((3, 5), 55.72, 0)]</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[((3, 4), 47.76, 0), ((3, 4), 55.72, 0)]</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>63.67999999999999</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>35.81999999999999</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -826,14 +806,8 @@
           <t>((1, 3), 4)</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>73.63</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>[((3, 5), 47.76, 0), ((3, 5), 55.72, 0)]</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
@@ -843,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -852,9 +826,7 @@
           <t>((1, 3), 5)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>79.59999999999999</v>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
@@ -875,23 +847,23 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9.800000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0), ((1, 3), 8.6, 0), ((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0)]</t>
+          <t>[((1, 3), 4.0, 0), ((1, 3), 4.2, 0), ((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0), ((1, 3), 6.0, 0), ((1, 3), 6.2, 0), ((1, 3), 6.4, 0), ((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0)]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>9.000000000000007</v>
+        <v>38</v>
       </c>
       <c r="G17" t="n">
-        <v>119.4</v>
+        <v>321.5999999999998</v>
       </c>
       <c r="H17" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -901,24 +873,20 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>15.77</v>
+        <v>13.77</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0), ((1, 3), 8.6, 0), ((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>[((2, 3), 8.0, 0), ((2, 3), 8.2, 0), ((2, 3), 8.4, 0), ((2, 3), 8.6, 0), ((2, 3), 8.8, 0), ((2, 3), 9.0, 0), ((2, 3), 9.2, 0), ((2, 3), 9.4, 0), ((2, 3), 9.6, 0), ((2, 3), 9.8, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 4.0, 0), ((1, 3), 4.2, 0), ((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0), ((1, 3), 6.0, 0), ((1, 3), 6.2, 0), ((1, 3), 6.4, 0), ((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>68.7</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>1</v>
@@ -931,19 +899,27 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21.74</v>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+        <v>23.88</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>[((3, 5), 15.92, 0), ((3, 5), 23.88, 0)]</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>[((3, 4), 15.92, 0), ((3, 4), 23.88, 0)]</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>15.92</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>107.42</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20">
@@ -952,18 +928,28 @@
           <t>((2, 1), 4)</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>47.75</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>[((3, 5), 15.92, 0), ((3, 5), 23.88, 0)]</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>[((4, 5), 47.75, 0)]</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="21">
@@ -972,7 +958,9 @@
           <t>((2, 1), 5)</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>53.72</v>
+      </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -993,23 +981,23 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>28.2</v>
+        <v>54.8</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
+          <t>[((1, 3), 51.0, 0), ((1, 3), 51.2, 0), ((1, 3), 51.4, 0), ((1, 3), 51.6, 0), ((1, 3), 51.8, 0), ((1, 3), 52.0, 0), ((1, 3), 52.2, 0), ((1, 3), 52.4, 0), ((1, 3), 52.6, 0), ((1, 3), 52.8, 0), ((1, 3), 53.0, 0), ((1, 3), 53.2, 0), ((1, 3), 53.4, 0), ((1, 3), 53.6, 0), ((1, 3), 53.8, 0), ((1, 3), 54.0, 0), ((1, 3), 54.2, 0), ((1, 3), 54.4, 0), ((1, 3), 54.6, 0), ((1, 3), 54.8, 0)]</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>8.999999999999993</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G22" t="n">
-        <v>131.7</v>
+        <v>238.8</v>
       </c>
       <c r="H22" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1019,24 +1007,20 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>35.4</v>
+        <v>60.77</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>[((2, 3), 33.6, 0), ((2, 3), 33.8, 0), ((2, 3), 34.0, 0), ((2, 3), 34.2, 0), ((2, 3), 34.4, 0), ((2, 3), 34.6, 0), ((2, 3), 34.8, 0), ((2, 3), 35.0, 0), ((2, 3), 35.2, 0), ((2, 3), 35.4, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 51.0, 0), ((1, 3), 51.2, 0), ((1, 3), 51.4, 0), ((1, 3), 51.6, 0), ((1, 3), 51.8, 0), ((1, 3), 52.0, 0), ((1, 3), 52.2, 0), ((1, 3), 52.4, 0), ((1, 3), 52.6, 0), ((1, 3), 52.8, 0), ((1, 3), 53.0, 0), ((1, 3), 53.2, 0), ((1, 3), 53.4, 0), ((1, 3), 53.6, 0), ((1, 3), 53.8, 0), ((1, 3), 54.0, 0), ((1, 3), 54.2, 0), ((1, 3), 54.4, 0), ((1, 3), 54.6, 0), ((1, 3), 54.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>8.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
@@ -1049,7 +1033,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>41.37</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
@@ -1107,85 +1091,107 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>((2, 3), 1)</t>
+          <t>((3, 1), 1)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>48.6</v>
+        <v>10</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[((1, 3), 46.8, 0), ((1, 3), 47.0, 0), ((1, 3), 47.2, 0), ((1, 3), 47.4, 0), ((1, 3), 47.6, 0), ((1, 3), 47.8, 0), ((1, 3), 48.0, 0), ((1, 3), 48.2, 0), ((1, 3), 48.4, 0), ((1, 3), 48.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
+          <t>[((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0), ((1, 3), 8.6, 0), ((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0), ((1, 3), 10.0, 0)]</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>[((1, 2), 0, 0), ((1, 2), 7.96, 0)]</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>9.000000000000014</v>
+        <v>23.04</v>
       </c>
       <c r="G27" t="n">
-        <v>119.4</v>
+        <v>339.7400000000001</v>
       </c>
       <c r="H27" t="n">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>((2, 3), 2)</t>
+          <t>((3, 1), 2)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>54.57</v>
+        <v>15.97</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[((1, 3), 46.8, 0), ((1, 3), 47.0, 0), ((1, 3), 47.2, 0), ((1, 3), 47.4, 0), ((1, 3), 47.6, 0), ((1, 3), 47.8, 0), ((1, 3), 48.0, 0), ((1, 3), 48.2, 0), ((1, 3), 48.4, 0), ((1, 3), 48.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
+          <t>[((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0), ((1, 3), 8.6, 0), ((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0), ((1, 3), 10.0, 0)]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>[((2, 3), 0, 0), ((2, 3), 0.2, 0), ((2, 3), 0.4, 0), ((2, 3), 0.6, 0), ((2, 3), 0.8, 0), ((2, 3), 1.0, 0), ((2, 3), 1.2, 0), ((2, 3), 1.4, 0), ((2, 3), 1.6, 0)]</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>136.53</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>214.47</v>
       </c>
       <c r="H28" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>((2, 3), 3)</t>
+          <t>((3, 1), 3)</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>60.54</v>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+        <v>39.8</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>[((3, 5), 31.84, 0), ((3, 5), 39.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>[((3, 4), 31.84, 0), ((3, 4), 39.8, 0)]</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>15.91999999999999</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>35.82000000000002</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>((2, 3), 4)</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
+          <t>((3, 1), 4)</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>45.77</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>[((3, 5), 31.84, 0), ((3, 5), 39.8, 0)]</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
@@ -1195,16 +1201,18 @@
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>((2, 3), 5)</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
+          <t>((3, 1), 5)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>51.74</v>
+      </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
@@ -1221,58 +1229,50 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>((3, 1), 1)</t>
+          <t>((3, 2), 1)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10</v>
+        <v>58.8</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.0, 0)]</t>
+          <t>[((1, 3), 55.0, 0), ((1, 3), 55.2, 0), ((1, 3), 55.4, 0), ((1, 3), 55.6, 0), ((1, 3), 55.8, 0), ((1, 3), 56.0, 0), ((1, 3), 56.2, 0), ((1, 3), 56.4, 0), ((1, 3), 56.6, 0), ((1, 3), 56.8, 0), ((1, 3), 57.0, 0), ((1, 3), 57.2, 0), ((1, 3), 57.4, 0), ((1, 3), 57.6, 0), ((1, 3), 57.8, 0), ((1, 3), 58.0, 0), ((1, 3), 58.2, 0), ((1, 3), 58.4, 0), ((1, 3), 58.6, 0), ((1, 3), 58.8, 0)]</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G32" t="n">
-        <v>11.94</v>
+        <v>238.8</v>
       </c>
       <c r="H32" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>((3, 1), 2)</t>
+          <t>((3, 2), 2)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>15.97</v>
+        <v>64.77</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.0, 0)]</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>[((2, 3), 10.0, 0)]</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>[((2, 3), 10.2, 0), ((2, 3), 10.4, 0), ((2, 3), 10.6, 0), ((2, 3), 10.8, 0), ((2, 3), 11.0, 0), ((2, 3), 11.2, 0), ((2, 3), 11.4, 0), ((2, 3), 11.6, 0), ((2, 3), 11.8, 0), ((2, 3), 12.0, 0), ((2, 3), 12.2, 0), ((2, 3), 12.4, 0), ((2, 3), 12.6, 0), ((2, 3), 12.8, 0), ((2, 3), 13.0, 0), ((2, 3), 13.2, 0), ((2, 3), 13.4, 0), ((2, 3), 13.6, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 55.0, 0), ((1, 3), 55.2, 0), ((1, 3), 55.4, 0), ((1, 3), 55.6, 0), ((1, 3), 55.8, 0), ((1, 3), 56.0, 0), ((1, 3), 56.2, 0), ((1, 3), 56.4, 0), ((1, 3), 56.6, 0), ((1, 3), 56.8, 0), ((1, 3), 57.0, 0), ((1, 3), 57.2, 0), ((1, 3), 57.4, 0), ((1, 3), 57.6, 0), ((1, 3), 57.8, 0), ((1, 3), 58.0, 0), ((1, 3), 58.2, 0), ((1, 3), 58.4, 0), ((1, 3), 58.6, 0), ((1, 3), 58.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>79.23000000000002</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>113.43</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>1</v>
@@ -1281,11 +1281,11 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>((3, 1), 3)</t>
+          <t>((3, 2), 3)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>21.94</v>
+        <v>70.73999999999999</v>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
@@ -1303,7 +1303,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>((3, 1), 4)</t>
+          <t>((3, 2), 4)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1323,7 +1323,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>((3, 1), 5)</t>
+          <t>((3, 2), 5)</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1343,54 +1343,50 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>((3, 2), 1)</t>
+          <t>((4, 1), 1)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>30.2</v>
+        <v>14</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[((1, 3), 28.4, 0), ((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0)]</t>
+          <t>[((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0), ((1, 3), 10.8, 0), ((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0), ((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0), ((1, 3), 13.0, 0), ((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0)]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>8.999999999999993</v>
+        <v>38</v>
       </c>
       <c r="G37" t="n">
-        <v>131.7</v>
+        <v>834.4000000000003</v>
       </c>
       <c r="H37" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>((3, 2), 2)</t>
+          <t>((4, 1), 2)</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>37.4</v>
+        <v>19.97</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[((1, 3), 28.4, 0), ((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>[((2, 3), 35.6, 0), ((2, 3), 35.8, 0), ((2, 3), 36.0, 0), ((2, 3), 36.2, 0), ((2, 3), 36.4, 0), ((2, 3), 36.6, 0), ((2, 3), 36.8, 0), ((2, 3), 37.0, 0), ((2, 3), 37.2, 0), ((2, 3), 37.4, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0), ((1, 3), 10.8, 0), ((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0), ((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0), ((1, 3), 13.0, 0), ((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0)]</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>8.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
         <v>1</v>
@@ -1399,33 +1395,47 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>((3, 2), 3)</t>
+          <t>((4, 1), 3)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>43.37</v>
-      </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+        <v>55.72</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>[((3, 5), 47.76, 0), ((3, 5), 55.72, 0)]</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>[((3, 4), 47.76, 0), ((3, 4), 55.72, 0)]</t>
+        </is>
+      </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>15.92</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>35.81999999999999</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>((3, 2), 4)</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
+          <t>((4, 1), 4)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>61.69</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>[((3, 5), 47.76, 0), ((3, 5), 55.72, 0)]</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
@@ -1435,16 +1445,18 @@
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>((3, 2), 5)</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
+          <t>((4, 1), 5)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>67.66</v>
+      </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
@@ -1461,41 +1473,41 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 1)</t>
+          <t>((5, 1), 1)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>50.6</v>
+        <v>18</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[((1, 3), 48.8, 0), ((1, 3), 49.0, 0), ((1, 3), 49.2, 0), ((1, 3), 49.4, 0), ((1, 3), 49.6, 0), ((1, 3), 49.8, 0), ((1, 3), 50.0, 0), ((1, 3), 50.2, 0), ((1, 3), 50.4, 0), ((1, 3), 50.6, 0)]</t>
+          <t>[((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0), ((1, 3), 15.2, 0), ((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0), ((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0), ((1, 3), 17.4, 0), ((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0)]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>9.000000000000014</v>
+        <v>38</v>
       </c>
       <c r="G42" t="n">
-        <v>119.4</v>
+        <v>238.8</v>
       </c>
       <c r="H42" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 2)</t>
+          <t>((5, 1), 2)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>56.57</v>
+        <v>23.97</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[((1, 3), 48.8, 0), ((1, 3), 49.0, 0), ((1, 3), 49.2, 0), ((1, 3), 49.4, 0), ((1, 3), 49.6, 0), ((1, 3), 49.8, 0), ((1, 3), 50.0, 0), ((1, 3), 50.2, 0), ((1, 3), 50.4, 0), ((1, 3), 50.6, 0)]</t>
+          <t>[((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0), ((1, 3), 15.2, 0), ((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0), ((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0), ((1, 3), 17.4, 0), ((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0)]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -1507,17 +1519,17 @@
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 3)</t>
+          <t>((5, 1), 3)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>62.54</v>
+        <v>29.94</v>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
@@ -1535,7 +1547,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 4)</t>
+          <t>((5, 1), 4)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1555,7 +1567,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 5)</t>
+          <t>((5, 1), 5)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1575,54 +1587,58 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 1)</t>
+          <t>((5, 2), 1)</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>12</v>
+        <v>39.8</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0), ((1, 3), 10.8, 0), ((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0)]</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr"/>
+          <t>[((1, 3), 28.4, 0), ((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0), ((1, 3), 30.4, 0)]</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>[((1, 2), 31.84, 0), ((1, 2), 39.8, 0)]</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>9</v>
+        <v>122.3599999999999</v>
       </c>
       <c r="G47" t="n">
-        <v>119.4</v>
+        <v>143.28</v>
       </c>
       <c r="H47" t="n">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 2)</t>
+          <t>((5, 2), 2)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>17.97</v>
+        <v>45.77</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0), ((1, 3), 10.8, 0), ((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0)]</t>
+          <t>[((1, 3), 28.4, 0), ((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0), ((1, 3), 30.4, 0)]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[((2, 3), 13.8, 0), ((2, 3), 14.0, 0), ((2, 3), 14.2, 0), ((2, 3), 14.4, 0), ((2, 3), 14.6, 0), ((2, 3), 14.8, 0), ((2, 3), 15.0, 0), ((2, 3), 15.2, 0), ((2, 3), 15.4, 0), ((2, 3), 15.6, 0)]</t>
+          <t>[((2, 3), 3.6, 0), ((2, 3), 3.8, 0), ((2, 3), 4.0, 0), ((2, 3), 4.2, 0), ((2, 3), 4.4, 0), ((2, 3), 4.6, 0), ((2, 3), 4.8, 0), ((2, 3), 5.0, 0), ((2, 3), 5.2, 0)]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
-        <v>32.69999999999999</v>
+        <v>372.33</v>
       </c>
       <c r="G48" t="n">
-        <v>59.70000000000002</v>
+        <v>53.72999999999999</v>
       </c>
       <c r="H48" t="n">
         <v>1</v>
@@ -1631,11 +1647,11 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 3)</t>
+          <t>((5, 2), 3)</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>23.94</v>
+        <v>51.74</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
@@ -1653,7 +1669,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 4)</t>
+          <t>((5, 2), 4)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1673,7 +1689,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 5)</t>
+          <t>((5, 2), 5)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1693,58 +1709,58 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 1)</t>
+          <t>((5, 3), 1)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>30.4</v>
+        <v>59.8</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.4, 0)]</t>
+          <t>[((1, 3), 59.0, 0), ((1, 3), 59.2, 0), ((1, 3), 59.4, 0), ((1, 3), 59.6, 0), ((1, 3), 59.8, 0)]</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>1.999999999999986</v>
       </c>
       <c r="G52" t="n">
-        <v>16.77</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="H52" t="n">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 2)</t>
+          <t>((5, 3), 2)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>41.2</v>
+        <v>65.77</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.4, 0)]</t>
+          <t>[((1, 3), 59.0, 0), ((1, 3), 59.2, 0), ((1, 3), 59.4, 0), ((1, 3), 59.6, 0), ((1, 3), 59.8, 0)]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[((2, 3), 37.6, 0), ((2, 3), 37.8, 0), ((2, 3), 38.0, 0), ((2, 3), 38.2, 0), ((2, 3), 38.4, 0), ((2, 3), 38.6, 0), ((2, 3), 38.8, 0), ((2, 3), 39.0, 0), ((2, 3), 39.2, 0), ((2, 3), 39.4, 0), ((2, 3), 39.6, 0), ((2, 3), 39.8, 0), ((2, 3), 40.0, 0), ((2, 3), 40.2, 0), ((2, 3), 40.4, 0), ((2, 3), 40.6, 0)]</t>
+          <t>[((2, 3), 9.0, 0), ((2, 3), 9.2, 0), ((2, 3), 9.4, 0), ((2, 3), 9.6, 0), ((2, 3), 9.8, 0), ((2, 3), 10.0, 0)]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[((2, 3), 40.8, 0), ((2, 3), 41.0, 0), ((2, 3), 41.2, 0)]</t>
+          <t>[((2, 3), 10.2, 0), ((2, 3), 10.4, 0), ((2, 3), 10.6, 0), ((2, 3), 10.8, 0), ((2, 3), 11.0, 0), ((2, 3), 11.2, 0), ((2, 3), 11.4, 0), ((2, 3), 11.6, 0), ((2, 3), 11.8, 0)]</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>34.20000000000005</v>
+        <v>830.55</v>
       </c>
       <c r="G53" t="n">
-        <v>113.43</v>
+        <v>89.54999999999998</v>
       </c>
       <c r="H53" t="n">
         <v>1</v>
@@ -1753,11 +1769,11 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 3)</t>
+          <t>((5, 3), 3)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>47.17</v>
+        <v>71.73999999999999</v>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
@@ -1775,7 +1791,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 4)</t>
+          <t>((5, 3), 4)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1795,7 +1811,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 5)</t>
+          <t>((5, 3), 5)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1815,63 +1831,71 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 1)</t>
+          <t>((6, 1), 1)</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>54.8</v>
+        <v>23.88</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[((1, 3), 53.0, 0), ((1, 3), 53.2, 0), ((1, 3), 53.4, 0), ((1, 3), 53.6, 0), ((1, 3), 53.8, 0), ((1, 3), 54.0, 0), ((1, 3), 54.2, 0), ((1, 3), 54.4, 0), ((1, 3), 54.6, 0), ((1, 3), 54.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
+          <t>[((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0), ((1, 3), 19.6, 0), ((1, 3), 19.8, 0), ((1, 3), 20.0, 0), ((1, 3), 20.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>[((1, 2), 15.92, 0), ((1, 2), 23.88, 0)]</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
-        <v>8.999999999999972</v>
+        <v>59.43999999999998</v>
       </c>
       <c r="G57" t="n">
-        <v>119.4</v>
+        <v>143.28</v>
       </c>
       <c r="H57" t="n">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 2)</t>
+          <t>((6, 1), 2)</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>60.77</v>
+        <v>29.85</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[((1, 3), 53.0, 0), ((1, 3), 53.2, 0), ((1, 3), 53.4, 0), ((1, 3), 53.6, 0), ((1, 3), 53.8, 0), ((1, 3), 54.0, 0), ((1, 3), 54.2, 0), ((1, 3), 54.4, 0), ((1, 3), 54.6, 0), ((1, 3), 54.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
+          <t>[((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0), ((1, 3), 19.6, 0), ((1, 3), 19.8, 0), ((1, 3), 20.0, 0), ((1, 3), 20.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>[((2, 3), 1.8, 0), ((2, 3), 2.0, 0), ((2, 3), 2.2, 0), ((2, 3), 2.4, 0), ((2, 3), 2.6, 0), ((2, 3), 2.8, 0), ((2, 3), 3.0, 0), ((2, 3), 3.2, 0), ((2, 3), 3.4, 0)]</t>
+        </is>
+      </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>245.25</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>53.72999999999999</v>
       </c>
       <c r="H58" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 3)</t>
+          <t>((6, 1), 3)</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>66.73999999999999</v>
+        <v>35.82</v>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
@@ -1889,7 +1913,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 4)</t>
+          <t>((6, 1), 4)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1909,7 +1933,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 5)</t>
+          <t>((6, 1), 5)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1929,54 +1953,50 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 1)</t>
+          <t>((6, 2), 1)</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>14</v>
+        <v>44.6</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0), ((1, 3), 13.0, 0), ((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0)]</t>
+          <t>[((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0), ((1, 3), 41.6, 0), ((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0), ((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0), ((1, 3), 43.8, 0), ((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0)]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="n">
-        <v>9</v>
+        <v>38.00000000000003</v>
       </c>
       <c r="G62" t="n">
-        <v>119.4</v>
+        <v>238.8</v>
       </c>
       <c r="H62" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 2)</t>
+          <t>((6, 2), 2)</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>19.97</v>
+        <v>50.57</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0), ((1, 3), 13.0, 0), ((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0)]</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>[((2, 3), 15.8, 0), ((2, 3), 16.0, 0), ((2, 3), 16.2, 0), ((2, 3), 16.4, 0), ((2, 3), 16.6, 0), ((2, 3), 16.8, 0), ((2, 3), 17.0, 0), ((2, 3), 17.2, 0), ((2, 3), 17.4, 0), ((2, 3), 17.6, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0), ((1, 3), 41.6, 0), ((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0), ((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0), ((1, 3), 43.8, 0), ((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0)]</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="n">
-        <v>32.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>59.70000000000002</v>
+        <v>0</v>
       </c>
       <c r="H63" t="n">
         <v>1</v>
@@ -1985,11 +2005,11 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 3)</t>
+          <t>((6, 2), 3)</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>25.94</v>
+        <v>56.54</v>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
@@ -2007,7 +2027,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 4)</t>
+          <t>((6, 2), 4)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -2027,7 +2047,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 5)</t>
+          <t>((6, 2), 5)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -2047,54 +2067,50 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 1)</t>
+          <t>((7, 1), 1)</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>34.4</v>
+        <v>24.2</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[((1, 3), 32.6, 0), ((1, 3), 32.8, 0), ((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0)]</t>
+          <t>[((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0), ((1, 3), 21.8, 0), ((1, 3), 22.0, 0), ((1, 3), 22.2, 0), ((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0), ((1, 3), 24.0, 0), ((1, 3), 24.2, 0)]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="n">
-        <v>8.999999999999986</v>
+        <v>37.99999999999997</v>
       </c>
       <c r="G67" t="n">
-        <v>167.7000000000001</v>
+        <v>238.8</v>
       </c>
       <c r="H67" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 2)</t>
+          <t>((7, 1), 2)</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>45.2</v>
+        <v>30.17</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[((1, 3), 32.6, 0), ((1, 3), 32.8, 0), ((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0)]</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>[((2, 3), 43.4, 0), ((2, 3), 43.6, 0), ((2, 3), 43.8, 0), ((2, 3), 44.0, 0), ((2, 3), 44.2, 0), ((2, 3), 44.4, 0), ((2, 3), 44.6, 0), ((2, 3), 44.8, 0), ((2, 3), 45.0, 0), ((2, 3), 45.2, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0), ((1, 3), 21.8, 0), ((1, 3), 22.0, 0), ((1, 3), 22.2, 0), ((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0), ((1, 3), 24.0, 0), ((1, 3), 24.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="n">
-        <v>9.000000000000028</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="H68" t="n">
         <v>1</v>
@@ -2103,11 +2119,11 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 3)</t>
+          <t>((7, 1), 3)</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>51.17</v>
+        <v>36.14</v>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
@@ -2125,7 +2141,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 4)</t>
+          <t>((7, 1), 4)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2145,7 +2161,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 5)</t>
+          <t>((7, 1), 5)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2165,41 +2181,41 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 1)</t>
+          <t>((7, 2), 1)</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>58.8</v>
+        <v>48.6</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[((1, 3), 57.0, 0), ((1, 3), 57.2, 0), ((1, 3), 57.4, 0), ((1, 3), 57.6, 0), ((1, 3), 57.8, 0), ((1, 3), 58.0, 0), ((1, 3), 58.2, 0), ((1, 3), 58.4, 0), ((1, 3), 58.6, 0), ((1, 3), 58.8, 0)]</t>
+          <t>[((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0), ((1, 3), 46.0, 0), ((1, 3), 46.2, 0), ((1, 3), 46.4, 0), ((1, 3), 46.6, 0), ((1, 3), 46.8, 0), ((1, 3), 47.0, 0), ((1, 3), 47.2, 0), ((1, 3), 47.4, 0), ((1, 3), 47.6, 0), ((1, 3), 47.8, 0), ((1, 3), 48.0, 0), ((1, 3), 48.2, 0), ((1, 3), 48.4, 0), ((1, 3), 48.6, 0)]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="n">
-        <v>8.999999999999972</v>
+        <v>38.00000000000003</v>
       </c>
       <c r="G72" t="n">
-        <v>119.4</v>
+        <v>238.8</v>
       </c>
       <c r="H72" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 2)</t>
+          <t>((7, 2), 2)</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>64.77</v>
+        <v>54.57</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[((1, 3), 57.0, 0), ((1, 3), 57.2, 0), ((1, 3), 57.4, 0), ((1, 3), 57.6, 0), ((1, 3), 57.8, 0), ((1, 3), 58.0, 0), ((1, 3), 58.2, 0), ((1, 3), 58.4, 0), ((1, 3), 58.6, 0), ((1, 3), 58.8, 0)]</t>
+          <t>[((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0), ((1, 3), 46.0, 0), ((1, 3), 46.2, 0), ((1, 3), 46.4, 0), ((1, 3), 46.6, 0), ((1, 3), 46.8, 0), ((1, 3), 47.0, 0), ((1, 3), 47.2, 0), ((1, 3), 47.4, 0), ((1, 3), 47.6, 0), ((1, 3), 47.8, 0), ((1, 3), 48.0, 0), ((1, 3), 48.2, 0), ((1, 3), 48.4, 0), ((1, 3), 48.6, 0)]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -2211,17 +2227,17 @@
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 3)</t>
+          <t>((7, 2), 3)</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>70.73999999999999</v>
+        <v>60.54</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
@@ -2239,7 +2255,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 4)</t>
+          <t>((7, 2), 4)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2259,7 +2275,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 5)</t>
+          <t>((7, 2), 5)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2279,54 +2295,50 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 1)</t>
+          <t>((8, 1), 1)</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>16</v>
+        <v>34.4</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0), ((1, 3), 15.2, 0), ((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0)]</t>
+          <t>[((1, 3), 30.6, 0), ((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0), ((1, 3), 32.6, 0), ((1, 3), 32.8, 0), ((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0)]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="n">
-        <v>9</v>
+        <v>37.99999999999996</v>
       </c>
       <c r="G77" t="n">
-        <v>119.4</v>
+        <v>238.8</v>
       </c>
       <c r="H77" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 2)</t>
+          <t>((8, 1), 2)</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>21.97</v>
+        <v>40.37</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>[((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0), ((1, 3), 15.2, 0), ((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0)]</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>[((2, 3), 17.8, 0), ((2, 3), 18.0, 0), ((2, 3), 18.2, 0), ((2, 3), 18.4, 0), ((2, 3), 18.6, 0), ((2, 3), 18.8, 0), ((2, 3), 19.0, 0), ((2, 3), 19.2, 0), ((2, 3), 19.4, 0), ((2, 3), 19.6, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 30.6, 0), ((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0), ((1, 3), 32.6, 0), ((1, 3), 32.8, 0), ((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0)]</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="n">
-        <v>32.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>59.70000000000002</v>
+        <v>0</v>
       </c>
       <c r="H78" t="n">
         <v>1</v>
@@ -2335,11 +2347,11 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 3)</t>
+          <t>((8, 1), 3)</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>27.94</v>
+        <v>46.34</v>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
@@ -2357,7 +2369,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 4)</t>
+          <t>((8, 1), 4)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -2377,7 +2389,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 5)</t>
+          <t>((8, 1), 5)</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -2397,54 +2409,44 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>36.4</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>[((1, 3), 34.6, 0), ((1, 3), 34.8, 0), ((1, 3), 35.0, 0), ((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0)]</t>
-        </is>
-      </c>
+          <t>((8, 2), 1)</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="n">
-        <v>8.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>167.7000000000001</v>
+        <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 2)</t>
+          <t>((8, 2), 2)</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>47.2</v>
+        <v>55.8</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>[((1, 3), 34.6, 0), ((1, 3), 34.8, 0), ((1, 3), 35.0, 0), ((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0)]</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>[((2, 3), 45.4, 0), ((2, 3), 45.6, 0), ((2, 3), 45.8, 0), ((2, 3), 46.0, 0), ((2, 3), 46.2, 0), ((2, 3), 46.4, 0), ((2, 3), 46.6, 0), ((2, 3), 46.8, 0), ((2, 3), 47.0, 0), ((2, 3), 47.2, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 52.0, 0), ((2, 3), 52.2, 0), ((2, 3), 52.4, 0), ((2, 3), 52.6, 0), ((2, 3), 52.8, 0), ((2, 3), 53.0, 0), ((2, 3), 53.2, 0), ((2, 3), 53.4, 0), ((2, 3), 53.6, 0), ((2, 3), 53.8, 0), ((2, 3), 54.0, 0), ((2, 3), 54.2, 0), ((2, 3), 54.4, 0), ((2, 3), 54.6, 0), ((2, 3), 54.8, 0), ((2, 3), 55.0, 0), ((2, 3), 55.2, 0), ((2, 3), 55.4, 0), ((2, 3), 55.6, 0), ((2, 3), 55.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="n">
-        <v>9.000000000000028</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G83" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4000000000001</v>
       </c>
       <c r="H83" t="n">
         <v>1</v>
@@ -2453,11 +2455,11 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 3)</t>
+          <t>((8, 2), 3)</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>53.17</v>
+        <v>61.77</v>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
@@ -2475,7 +2477,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 4)</t>
+          <t>((8, 2), 4)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2495,7 +2497,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 5)</t>
+          <t>((8, 2), 5)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2515,41 +2517,41 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 1)</t>
+          <t>((9, 1), 1)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>59.8</v>
+        <v>38.4</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>[((1, 3), 59.0, 0), ((1, 3), 59.2, 0), ((1, 3), 59.4, 0), ((1, 3), 59.6, 0), ((1, 3), 59.8, 0)]</t>
+          <t>[((1, 3), 34.6, 0), ((1, 3), 34.8, 0), ((1, 3), 35.0, 0), ((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0), ((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0), ((1, 3), 37.2, 0), ((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0)]</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="n">
-        <v>1.999999999999986</v>
+        <v>37.99999999999997</v>
       </c>
       <c r="G87" t="n">
-        <v>59.69999999999999</v>
+        <v>238.8</v>
       </c>
       <c r="H87" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 2)</t>
+          <t>((9, 1), 2)</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>65.77</v>
+        <v>44.37</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>[((1, 3), 59.0, 0), ((1, 3), 59.2, 0), ((1, 3), 59.4, 0), ((1, 3), 59.6, 0), ((1, 3), 59.8, 0)]</t>
+          <t>[((1, 3), 34.6, 0), ((1, 3), 34.8, 0), ((1, 3), 35.0, 0), ((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0), ((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0), ((1, 3), 37.2, 0), ((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0)]</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
@@ -2561,17 +2563,17 @@
         <v>0</v>
       </c>
       <c r="H88" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 3)</t>
+          <t>((9, 1), 3)</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>71.73999999999999</v>
+        <v>50.34</v>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
@@ -2589,7 +2591,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 4)</t>
+          <t>((9, 1), 4)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2609,7 +2611,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 5)</t>
+          <t>((9, 1), 5)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2629,58 +2631,44 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>18</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>[((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0), ((1, 3), 17.4, 0), ((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0)]</t>
-        </is>
-      </c>
+          <t>((9, 2), 1)</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>119.4</v>
+        <v>0</v>
       </c>
       <c r="H92" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 2)</t>
+          <t>((9, 2), 2)</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>23.97</v>
+        <v>59.8</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>[((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0), ((1, 3), 17.4, 0), ((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0)]</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>[((2, 3), 19.8, 0), ((2, 3), 20.0, 0), ((2, 3), 20.2, 0)]</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>[((2, 3), 20.4, 0), ((2, 3), 20.6, 0), ((2, 3), 20.8, 0), ((2, 3), 21.0, 0), ((2, 3), 21.2, 0), ((2, 3), 21.4, 0), ((2, 3), 21.6, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 56.0, 0), ((2, 3), 56.2, 0), ((2, 3), 56.4, 0), ((2, 3), 56.6, 0), ((2, 3), 56.8, 0), ((2, 3), 57.0, 0), ((2, 3), 57.2, 0), ((2, 3), 57.4, 0), ((2, 3), 57.6, 0), ((2, 3), 57.8, 0), ((2, 3), 58.0, 0), ((2, 3), 58.2, 0), ((2, 3), 58.4, 0), ((2, 3), 58.6, 0), ((2, 3), 58.8, 0), ((2, 3), 59.0, 0), ((2, 3), 59.2, 0), ((2, 3), 59.4, 0), ((2, 3), 59.6, 0), ((2, 3), 59.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="inlineStr"/>
       <c r="F93" t="n">
-        <v>32.69999999999999</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G93" t="n">
-        <v>59.70000000000002</v>
+        <v>119.4</v>
       </c>
       <c r="H93" t="n">
         <v>1</v>
@@ -2689,11 +2677,11 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 3)</t>
+          <t>((9, 2), 3)</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>29.94</v>
+        <v>65.77</v>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
@@ -2711,7 +2699,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 4)</t>
+          <t>((9, 2), 4)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2731,7 +2719,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 5)</t>
+          <t>((9, 2), 5)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2751,54 +2739,54 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 1)</t>
+          <t>((10, 1), 1)</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>38.4</v>
+        <v>50.8</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>[((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0), ((1, 3), 37.2, 0), ((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0)]</t>
+          <t>[((1, 3), 48.8, 0), ((1, 3), 49.0, 0), ((1, 3), 49.2, 0), ((1, 3), 49.4, 0), ((1, 3), 49.6, 0), ((1, 3), 49.8, 0), ((1, 3), 50.0, 0), ((1, 3), 50.2, 0), ((1, 3), 50.4, 0), ((1, 3), 50.6, 0), ((1, 3), 50.8, 0)]</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="n">
-        <v>8.999999999999986</v>
+        <v>10.99999999999997</v>
       </c>
       <c r="G97" t="n">
-        <v>167.7000000000001</v>
+        <v>131.34</v>
       </c>
       <c r="H97" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 2)</t>
+          <t>((10, 1), 2)</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>49.2</v>
+        <v>56.77</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>[((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0), ((1, 3), 37.2, 0), ((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0)]</t>
+          <t>[((1, 3), 48.8, 0), ((1, 3), 49.0, 0), ((1, 3), 49.2, 0), ((1, 3), 49.4, 0), ((1, 3), 49.6, 0), ((1, 3), 49.8, 0), ((1, 3), 50.0, 0), ((1, 3), 50.2, 0), ((1, 3), 50.4, 0), ((1, 3), 50.6, 0), ((1, 3), 50.8, 0)]</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>[((2, 3), 47.4, 0), ((2, 3), 47.6, 0), ((2, 3), 47.8, 0), ((2, 3), 48.0, 0), ((2, 3), 48.2, 0), ((2, 3), 48.4, 0), ((2, 3), 48.6, 0), ((2, 3), 48.8, 0), ((2, 3), 49.0, 0), ((2, 3), 49.2, 0)]</t>
+          <t>[((2, 3), 7.2, 0), ((2, 3), 7.4, 0), ((2, 3), 7.6, 0), ((2, 3), 7.8, 0), ((2, 3), 8.0, 0), ((2, 3), 8.2, 0), ((2, 3), 8.4, 0), ((2, 3), 8.6, 0), ((2, 3), 8.8, 0)]</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="n">
-        <v>9.000000000000028</v>
+        <v>438.9300000000001</v>
       </c>
       <c r="G98" t="n">
-        <v>59.69999999999999</v>
+        <v>53.72999999999999</v>
       </c>
       <c r="H98" t="n">
         <v>1</v>
@@ -2807,11 +2795,11 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 3)</t>
+          <t>((10, 1), 3)</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>55.17</v>
+        <v>62.74</v>
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
@@ -2829,7 +2817,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 4)</t>
+          <t>((10, 1), 4)</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -2849,7 +2837,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 5)</t>
+          <t>((10, 1), 5)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2869,54 +2857,44 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B102" t="n">
-        <v>20</v>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>[((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0), ((1, 3), 19.6, 0), ((1, 3), 19.8, 0), ((1, 3), 20.0, 0)]</t>
-        </is>
-      </c>
+          <t>((11, 1), 1)</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>119.4</v>
+        <v>0</v>
       </c>
       <c r="H102" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 2)</t>
+          <t>((11, 1), 2)</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>25.97</v>
+        <v>15.8</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>[((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0), ((1, 3), 19.6, 0), ((1, 3), 19.8, 0), ((1, 3), 20.0, 0)]</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>[((2, 3), 21.8, 0), ((2, 3), 22.0, 0), ((2, 3), 22.2, 0), ((2, 3), 22.4, 0), ((2, 3), 22.6, 0), ((2, 3), 22.8, 0), ((2, 3), 23.0, 0), ((2, 3), 23.2, 0), ((2, 3), 23.4, 0), ((2, 3), 23.6, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 12.0, 0), ((2, 3), 12.2, 0), ((2, 3), 12.4, 0), ((2, 3), 12.6, 0), ((2, 3), 12.8, 0), ((2, 3), 13.0, 0), ((2, 3), 13.2, 0), ((2, 3), 13.4, 0), ((2, 3), 13.6, 0), ((2, 3), 13.8, 0), ((2, 3), 14.0, 0), ((2, 3), 14.2, 0), ((2, 3), 14.4, 0), ((2, 3), 14.6, 0), ((2, 3), 14.8, 0), ((2, 3), 15.0, 0), ((2, 3), 15.2, 0), ((2, 3), 15.4, 0), ((2, 3), 15.6, 0), ((2, 3), 15.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="n">
-        <v>32.69999999999999</v>
+        <v>38.00000000000001</v>
       </c>
       <c r="G103" t="n">
-        <v>59.70000000000002</v>
+        <v>119.4</v>
       </c>
       <c r="H103" t="n">
         <v>1</v>
@@ -2925,11 +2903,11 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 3)</t>
+          <t>((11, 1), 3)</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>31.94</v>
+        <v>21.77</v>
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
@@ -2947,7 +2925,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 4)</t>
+          <t>((11, 1), 4)</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2967,7 +2945,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 5)</t>
+          <t>((11, 1), 5)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2987,58 +2965,44 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B107" t="n">
-        <v>39.8</v>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>[((1, 3), 4.0, 0), ((1, 3), 4.2, 0), ((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>[((1, 2), 31.84, 0), ((1, 2), 39.8, 0)]</t>
-        </is>
-      </c>
+          <t>((11, 2), 1)</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="n">
-        <v>356.9599999999999</v>
+        <v>0</v>
       </c>
       <c r="G107" t="n">
-        <v>131.34</v>
+        <v>0</v>
       </c>
       <c r="H107" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 2)</t>
+          <t>((11, 2), 2)</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>45.77</v>
+        <v>27.8</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>[((1, 3), 4.0, 0), ((1, 3), 4.2, 0), ((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>[((2, 3), 4.0, 0), ((2, 3), 4.2, 0), ((2, 3), 4.4, 0), ((2, 3), 4.6, 0), ((2, 3), 4.8, 0), ((2, 3), 5.0, 0), ((2, 3), 5.2, 0), ((2, 3), 5.4, 0), ((2, 3), 5.6, 0), ((2, 3), 5.8, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 24.0, 0), ((2, 3), 24.2, 0), ((2, 3), 24.4, 0), ((2, 3), 24.6, 0), ((2, 3), 24.8, 0), ((2, 3), 25.0, 0), ((2, 3), 25.2, 0), ((2, 3), 25.4, 0), ((2, 3), 25.6, 0), ((2, 3), 25.8, 0), ((2, 3), 26.0, 0), ((2, 3), 26.2, 0), ((2, 3), 26.4, 0), ((2, 3), 26.6, 0), ((2, 3), 26.8, 0), ((2, 3), 27.0, 0), ((2, 3), 27.2, 0), ((2, 3), 27.4, 0), ((2, 3), 27.6, 0), ((2, 3), 27.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="n">
-        <v>408.7</v>
+        <v>38.00000000000001</v>
       </c>
       <c r="G108" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4</v>
       </c>
       <c r="H108" t="n">
         <v>1</v>
@@ -3047,47 +3011,33 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 3)</t>
+          <t>((11, 2), 3)</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>51.74</v>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>[((3, 5), 31.84, 0), ((3, 5), 39.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>[((3, 4), 31.84, 0), ((3, 4), 39.8, 0)]</t>
-        </is>
-      </c>
+        <v>33.77</v>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="n">
-        <v>63.68000000000001</v>
+        <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>35.81999999999999</v>
+        <v>0</v>
       </c>
       <c r="H109" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 4)</t>
-        </is>
-      </c>
-      <c r="B110" t="n">
-        <v>57.71</v>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>[((3, 5), 31.84, 0), ((3, 5), 39.8, 0)]</t>
-        </is>
-      </c>
+          <t>((11, 2), 4)</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="n">
@@ -3097,18 +3047,16 @@
         <v>0</v>
       </c>
       <c r="H110" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 5)</t>
-        </is>
-      </c>
-      <c r="B111" t="n">
-        <v>63.68</v>
-      </c>
+          <t>((11, 2), 5)</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
@@ -3125,54 +3073,44 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B112" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>[((1, 3), 20.2, 0)]</t>
-        </is>
-      </c>
+          <t>((11, 3), 1)</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="n">
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>13.17</v>
+        <v>0</v>
       </c>
       <c r="H112" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 2)</t>
+          <t>((11, 3), 2)</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>27.4</v>
+        <v>39.8</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>[((1, 3), 20.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>[((2, 3), 23.8, 0), ((2, 3), 24.0, 0), ((2, 3), 24.2, 0), ((2, 3), 24.4, 0), ((2, 3), 24.6, 0), ((2, 3), 24.8, 0), ((2, 3), 25.0, 0), ((2, 3), 25.2, 0), ((2, 3), 25.4, 0), ((2, 3), 25.6, 0), ((2, 3), 25.8, 0), ((2, 3), 26.0, 0), ((2, 3), 26.2, 0), ((2, 3), 26.4, 0), ((2, 3), 26.6, 0), ((2, 3), 26.8, 0), ((2, 3), 27.0, 0), ((2, 3), 27.2, 0), ((2, 3), 27.4, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 36.0, 0), ((2, 3), 36.2, 0), ((2, 3), 36.4, 0), ((2, 3), 36.6, 0), ((2, 3), 36.8, 0), ((2, 3), 37.0, 0), ((2, 3), 37.2, 0), ((2, 3), 37.4, 0), ((2, 3), 37.6, 0), ((2, 3), 37.8, 0), ((2, 3), 38.0, 0), ((2, 3), 38.2, 0), ((2, 3), 38.4, 0), ((2, 3), 38.6, 0), ((2, 3), 38.8, 0), ((2, 3), 39.0, 0), ((2, 3), 39.2, 0), ((2, 3), 39.4, 0), ((2, 3), 39.6, 0), ((2, 3), 39.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="n">
-        <v>34.19999999999997</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G113" t="n">
-        <v>113.43</v>
+        <v>119.4000000000001</v>
       </c>
       <c r="H113" t="n">
         <v>1</v>
@@ -3181,11 +3119,11 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 3)</t>
+          <t>((11, 3), 3)</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>33.37</v>
+        <v>45.77</v>
       </c>
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
@@ -3203,7 +3141,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 4)</t>
+          <t>((11, 3), 4)</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -3223,7 +3161,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 5)</t>
+          <t>((11, 3), 5)</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -3243,58 +3181,48 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B117" t="n">
-        <v>40.4</v>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>[((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0), ((1, 3), 39.4, 0), ((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0)]</t>
-        </is>
-      </c>
+          <t>((11, 4), 1)</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="n">
-        <v>8.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>167.7000000000001</v>
+        <v>0</v>
       </c>
       <c r="H117" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 2)</t>
+          <t>((11, 4), 2)</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>51.2</v>
+        <v>51.8</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>[((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0), ((1, 3), 39.4, 0), ((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0)]</t>
+          <t>[((2, 3), 48.0, 0), ((2, 3), 48.2, 0), ((2, 3), 48.4, 0), ((2, 3), 48.6, 0), ((2, 3), 48.8, 0), ((2, 3), 49.0, 0), ((2, 3), 49.2, 0), ((2, 3), 49.4, 0), ((2, 3), 49.6, 0), ((2, 3), 49.8, 0), ((2, 3), 50.0, 0), ((2, 3), 50.2, 0), ((2, 3), 50.4, 0), ((2, 3), 50.6, 0), ((2, 3), 50.8, 0)]</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>[((2, 3), 49.4, 0), ((2, 3), 49.6, 0), ((2, 3), 49.8, 0), ((2, 3), 50.0, 0), ((2, 3), 50.2, 0), ((2, 3), 50.4, 0), ((2, 3), 50.6, 0), ((2, 3), 50.8, 0)]</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>[((2, 3), 51.0, 0), ((2, 3), 51.2, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 51.0, 0), ((2, 3), 51.2, 0), ((2, 3), 51.4, 0), ((2, 3), 51.6, 0), ((2, 3), 51.8, 0)]</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
       <c r="F118" t="n">
-        <v>9.000000000000028</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G118" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4000000000001</v>
       </c>
       <c r="H118" t="n">
         <v>1</v>
@@ -3303,11 +3231,11 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 3)</t>
+          <t>((11, 4), 3)</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>57.17</v>
+        <v>57.77</v>
       </c>
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr"/>
@@ -3325,7 +3253,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 4)</t>
+          <t>((11, 4), 4)</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -3345,7 +3273,7 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 5)</t>
+          <t>((11, 4), 5)</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -3365,54 +3293,44 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B122" t="n">
-        <v>22.2</v>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>[((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0), ((1, 3), 21.8, 0), ((1, 3), 22.0, 0), ((1, 3), 22.2, 0)]</t>
-        </is>
-      </c>
+          <t>((12, 1), 1)</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="n">
-        <v>8.999999999999993</v>
+        <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>131.7</v>
+        <v>0</v>
       </c>
       <c r="H122" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 2)</t>
+          <t>((12, 1), 2)</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>29.4</v>
+        <v>19.8</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>[((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0), ((1, 3), 21.8, 0), ((1, 3), 22.0, 0), ((1, 3), 22.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>[((2, 3), 27.6, 0), ((2, 3), 27.8, 0), ((2, 3), 28.0, 0), ((2, 3), 28.2, 0), ((2, 3), 28.4, 0), ((2, 3), 28.6, 0), ((2, 3), 28.8, 0), ((2, 3), 29.0, 0), ((2, 3), 29.2, 0), ((2, 3), 29.4, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 16.0, 0), ((2, 3), 16.2, 0), ((2, 3), 16.4, 0), ((2, 3), 16.6, 0), ((2, 3), 16.8, 0), ((2, 3), 17.0, 0), ((2, 3), 17.2, 0), ((2, 3), 17.4, 0), ((2, 3), 17.6, 0), ((2, 3), 17.8, 0), ((2, 3), 18.0, 0), ((2, 3), 18.2, 0), ((2, 3), 18.4, 0), ((2, 3), 18.6, 0), ((2, 3), 18.8, 0), ((2, 3), 19.0, 0), ((2, 3), 19.2, 0), ((2, 3), 19.4, 0), ((2, 3), 19.6, 0), ((2, 3), 19.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="n">
-        <v>8.999999999999986</v>
+        <v>38.00000000000001</v>
       </c>
       <c r="G123" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4</v>
       </c>
       <c r="H123" t="n">
         <v>1</v>
@@ -3421,11 +3339,11 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 3)</t>
+          <t>((12, 1), 3)</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>35.37</v>
+        <v>25.77</v>
       </c>
       <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr"/>
@@ -3443,7 +3361,7 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 4)</t>
+          <t>((12, 1), 4)</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -3463,7 +3381,7 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 5)</t>
+          <t>((12, 1), 5)</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -3483,54 +3401,48 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B127" t="n">
-        <v>42.6</v>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>[((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0), ((1, 3), 41.6, 0), ((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0)]</t>
-        </is>
-      </c>
+          <t>((12, 2), 1)</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="inlineStr"/>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="n">
-        <v>9.000000000000014</v>
+        <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>203.7</v>
+        <v>0</v>
       </c>
       <c r="H127" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 2)</t>
+          <t>((12, 2), 2)</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>57</v>
+        <v>31.8</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>[((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0), ((1, 3), 41.6, 0), ((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0)]</t>
+          <t>[((2, 3), 28.0, 0), ((2, 3), 28.2, 0), ((2, 3), 28.4, 0), ((2, 3), 28.6, 0), ((2, 3), 28.8, 0), ((2, 3), 29.0, 0), ((2, 3), 29.2, 0), ((2, 3), 29.4, 0), ((2, 3), 29.6, 0), ((2, 3), 29.8, 0), ((2, 3), 30.0, 0), ((2, 3), 30.2, 0), ((2, 3), 30.4, 0)]</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>[((2, 3), 55.2, 0), ((2, 3), 55.4, 0), ((2, 3), 55.6, 0), ((2, 3), 55.8, 0), ((2, 3), 56.0, 0), ((2, 3), 56.2, 0), ((2, 3), 56.4, 0), ((2, 3), 56.6, 0), ((2, 3), 56.8, 0), ((2, 3), 57.0, 0)]</t>
+          <t>[((2, 3), 30.6, 0), ((2, 3), 30.8, 0), ((2, 3), 31.0, 0), ((2, 3), 31.2, 0), ((2, 3), 31.4, 0), ((2, 3), 31.6, 0), ((2, 3), 31.8, 0)]</t>
         </is>
       </c>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="n">
-        <v>9</v>
+        <v>38.00000000000001</v>
       </c>
       <c r="G128" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4</v>
       </c>
       <c r="H128" t="n">
         <v>1</v>
@@ -3539,11 +3451,11 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 3)</t>
+          <t>((12, 2), 3)</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>62.97</v>
+        <v>37.77</v>
       </c>
       <c r="C129" t="inlineStr"/>
       <c r="D129" t="inlineStr"/>
@@ -3561,7 +3473,7 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 4)</t>
+          <t>((12, 2), 4)</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -3581,7 +3493,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 5)</t>
+          <t>((12, 2), 5)</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -3601,58 +3513,48 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B132" t="n">
-        <v>23.88</v>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>[((1, 3), 2.0, 0), ((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>[((1, 2), 15.92, 0), ((1, 2), 23.88, 0)]</t>
-        </is>
-      </c>
+          <t>((12, 3), 1)</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="n">
-        <v>217.76</v>
+        <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>131.34</v>
+        <v>0</v>
       </c>
       <c r="H132" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 2)</t>
+          <t>((12, 3), 2)</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>29.85</v>
+        <v>43.8</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>[((1, 3), 2.0, 0), ((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0)]</t>
+          <t>[((2, 3), 40.0, 0), ((2, 3), 40.2, 0), ((2, 3), 40.4, 0), ((2, 3), 40.6, 0)]</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>[((2, 3), 2.0, 0), ((2, 3), 2.2, 0), ((2, 3), 2.4, 0), ((2, 3), 2.6, 0), ((2, 3), 2.8, 0), ((2, 3), 3.0, 0), ((2, 3), 3.2, 0), ((2, 3), 3.4, 0), ((2, 3), 3.6, 0), ((2, 3), 3.8, 0)]</t>
+          <t>[((2, 3), 40.8, 0), ((2, 3), 41.0, 0), ((2, 3), 41.2, 0), ((2, 3), 41.4, 0), ((2, 3), 41.6, 0), ((2, 3), 41.8, 0), ((2, 3), 42.0, 0), ((2, 3), 42.2, 0), ((2, 3), 42.4, 0), ((2, 3), 42.6, 0), ((2, 3), 42.8, 0), ((2, 3), 43.0, 0), ((2, 3), 43.2, 0), ((2, 3), 43.4, 0), ((2, 3), 43.6, 0), ((2, 3), 43.8, 0)]</t>
         </is>
       </c>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="n">
-        <v>269.5</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G133" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4000000000001</v>
       </c>
       <c r="H133" t="n">
         <v>1</v>
@@ -3661,72 +3563,52 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 3)</t>
+          <t>((12, 3), 3)</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>35.82</v>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>[((3, 5), 15.92, 0), ((3, 5), 23.88, 0)]</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>[((3, 4), 15.92, 0), ((3, 4), 23.88, 0)]</t>
-        </is>
-      </c>
+        <v>49.77</v>
+      </c>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="n">
-        <v>63.67999999999999</v>
+        <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>59.66</v>
+        <v>0</v>
       </c>
       <c r="H134" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 4)</t>
-        </is>
-      </c>
-      <c r="B135" t="n">
-        <v>47.75</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>[((3, 5), 15.92, 0), ((3, 5), 23.88, 0)]</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>[((4, 5), 47.75, 0)]</t>
-        </is>
-      </c>
+          <t>((12, 3), 4)</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
       <c r="E135" t="inlineStr"/>
       <c r="F135" t="n">
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>5.969999999999999</v>
+        <v>0</v>
       </c>
       <c r="H135" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 5)</t>
-        </is>
-      </c>
-      <c r="B136" t="n">
-        <v>53.72</v>
-      </c>
+          <t>((12, 3), 5)</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr"/>
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="inlineStr"/>
@@ -3743,63 +3625,61 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B137" t="n">
-        <v>56.8</v>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>[((1, 3), 55.0, 0), ((1, 3), 55.2, 0), ((1, 3), 55.4, 0), ((1, 3), 55.6, 0), ((1, 3), 55.8, 0), ((1, 3), 56.0, 0), ((1, 3), 56.2, 0), ((1, 3), 56.4, 0), ((1, 3), 56.6, 0), ((1, 3), 56.8, 0)]</t>
-        </is>
-      </c>
+          <t>((13, 1), 1)</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="inlineStr"/>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="n">
-        <v>8.999999999999972</v>
+        <v>0</v>
       </c>
       <c r="G137" t="n">
-        <v>119.4</v>
+        <v>0</v>
       </c>
       <c r="H137" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 2)</t>
+          <t>((13, 1), 2)</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>62.77</v>
+        <v>23.8</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>[((1, 3), 55.0, 0), ((1, 3), 55.2, 0), ((1, 3), 55.4, 0), ((1, 3), 55.6, 0), ((1, 3), 55.8, 0), ((1, 3), 56.0, 0), ((1, 3), 56.2, 0), ((1, 3), 56.4, 0), ((1, 3), 56.6, 0), ((1, 3), 56.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr"/>
+          <t>[((2, 3), 20.0, 0), ((2, 3), 20.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>[((2, 3), 20.4, 0), ((2, 3), 20.6, 0), ((2, 3), 20.8, 0), ((2, 3), 21.0, 0), ((2, 3), 21.2, 0), ((2, 3), 21.4, 0), ((2, 3), 21.6, 0), ((2, 3), 21.8, 0), ((2, 3), 22.0, 0), ((2, 3), 22.2, 0), ((2, 3), 22.4, 0), ((2, 3), 22.6, 0), ((2, 3), 22.8, 0), ((2, 3), 23.0, 0), ((2, 3), 23.2, 0), ((2, 3), 23.4, 0), ((2, 3), 23.6, 0), ((2, 3), 23.8, 0)]</t>
+        </is>
+      </c>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="n">
-        <v>0</v>
+        <v>38.00000000000001</v>
       </c>
       <c r="G138" t="n">
-        <v>0</v>
+        <v>119.4</v>
       </c>
       <c r="H138" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 3)</t>
+          <t>((13, 1), 3)</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>68.73999999999999</v>
+        <v>29.77</v>
       </c>
       <c r="C139" t="inlineStr"/>
       <c r="D139" t="inlineStr"/>
@@ -3817,7 +3697,7 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 4)</t>
+          <t>((13, 1), 4)</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -3837,7 +3717,7 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 5)</t>
+          <t>((13, 1), 5)</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -3857,58 +3737,44 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B142" t="n">
-        <v>24.2</v>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>[((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0), ((1, 3), 24.0, 0), ((1, 3), 24.2, 0)]</t>
-        </is>
-      </c>
+          <t>((13, 2), 1)</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="n">
-        <v>8.999999999999993</v>
+        <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>131.7</v>
+        <v>0</v>
       </c>
       <c r="H142" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 2)</t>
+          <t>((13, 2), 2)</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>31.4</v>
+        <v>35.8</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>[((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0), ((1, 3), 24.0, 0), ((1, 3), 24.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>[((2, 3), 29.6, 0), ((2, 3), 29.8, 0), ((2, 3), 30.0, 0), ((2, 3), 30.2, 0), ((2, 3), 30.4, 0)]</t>
-        </is>
-      </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>[((2, 3), 30.6, 0), ((2, 3), 30.8, 0), ((2, 3), 31.0, 0), ((2, 3), 31.2, 0), ((2, 3), 31.4, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 32.0, 0), ((2, 3), 32.2, 0), ((2, 3), 32.4, 0), ((2, 3), 32.6, 0), ((2, 3), 32.8, 0), ((2, 3), 33.0, 0), ((2, 3), 33.2, 0), ((2, 3), 33.4, 0), ((2, 3), 33.6, 0), ((2, 3), 33.8, 0), ((2, 3), 34.0, 0), ((2, 3), 34.2, 0), ((2, 3), 34.4, 0), ((2, 3), 34.6, 0), ((2, 3), 34.8, 0), ((2, 3), 35.0, 0), ((2, 3), 35.2, 0), ((2, 3), 35.4, 0), ((2, 3), 35.6, 0), ((2, 3), 35.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="inlineStr"/>
       <c r="F143" t="n">
-        <v>8.999999999999986</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G143" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4000000000001</v>
       </c>
       <c r="H143" t="n">
         <v>1</v>
@@ -3917,11 +3783,11 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 3)</t>
+          <t>((13, 2), 3)</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>37.37</v>
+        <v>41.77</v>
       </c>
       <c r="C144" t="inlineStr"/>
       <c r="D144" t="inlineStr"/>
@@ -3939,7 +3805,7 @@
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 4)</t>
+          <t>((13, 2), 4)</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -3959,7 +3825,7 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 5)</t>
+          <t>((13, 2), 5)</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -3979,54 +3845,44 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B147" t="n">
-        <v>44.6</v>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>[((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0), ((1, 3), 43.8, 0), ((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0)]</t>
-        </is>
-      </c>
+          <t>((13, 3), 1)</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr"/>
       <c r="F147" t="n">
-        <v>9.000000000000014</v>
+        <v>0</v>
       </c>
       <c r="G147" t="n">
-        <v>203.7</v>
+        <v>0</v>
       </c>
       <c r="H147" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 2)</t>
+          <t>((13, 3), 2)</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>59</v>
+        <v>47.8</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>[((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0), ((1, 3), 43.8, 0), ((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>[((2, 3), 57.2, 0), ((2, 3), 57.4, 0), ((2, 3), 57.6, 0), ((2, 3), 57.8, 0), ((2, 3), 58.0, 0), ((2, 3), 58.2, 0), ((2, 3), 58.4, 0), ((2, 3), 58.6, 0), ((2, 3), 58.8, 0), ((2, 3), 59.0, 0)]</t>
-        </is>
-      </c>
+          <t>[((2, 3), 44.0, 0), ((2, 3), 44.2, 0), ((2, 3), 44.4, 0), ((2, 3), 44.6, 0), ((2, 3), 44.8, 0), ((2, 3), 45.0, 0), ((2, 3), 45.2, 0), ((2, 3), 45.4, 0), ((2, 3), 45.6, 0), ((2, 3), 45.8, 0), ((2, 3), 46.0, 0), ((2, 3), 46.2, 0), ((2, 3), 46.4, 0), ((2, 3), 46.6, 0), ((2, 3), 46.8, 0), ((2, 3), 47.0, 0), ((2, 3), 47.2, 0), ((2, 3), 47.4, 0), ((2, 3), 47.6, 0), ((2, 3), 47.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="n">
-        <v>9</v>
+        <v>37.99999999999994</v>
       </c>
       <c r="G148" t="n">
-        <v>59.69999999999999</v>
+        <v>119.4000000000001</v>
       </c>
       <c r="H148" t="n">
         <v>1</v>
@@ -4035,11 +3891,11 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 3)</t>
+          <t>((13, 3), 3)</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>64.97</v>
+        <v>53.77</v>
       </c>
       <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr"/>
@@ -4057,7 +3913,7 @@
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 4)</t>
+          <t>((13, 3), 4)</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
@@ -4077,7 +3933,7 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 5)</t>
+          <t>((13, 3), 5)</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -4094,588 +3950,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" s="1" t="inlineStr">
-        <is>
-          <t>((13, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B152" t="n">
-        <v>26.2</v>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>[((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0), ((1, 3), 26.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr"/>
-      <c r="E152" t="inlineStr"/>
-      <c r="F152" t="n">
-        <v>8.999999999999993</v>
-      </c>
-      <c r="G152" t="n">
-        <v>131.7</v>
-      </c>
-      <c r="H152" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="inlineStr">
-        <is>
-          <t>((13, 1), 2)</t>
-        </is>
-      </c>
-      <c r="B153" t="n">
-        <v>33.4</v>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>[((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0), ((1, 3), 26.2, 0)]</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>[((2, 3), 31.6, 0), ((2, 3), 31.8, 0), ((2, 3), 32.0, 0), ((2, 3), 32.2, 0), ((2, 3), 32.4, 0), ((2, 3), 32.6, 0), ((2, 3), 32.8, 0), ((2, 3), 33.0, 0), ((2, 3), 33.2, 0), ((2, 3), 33.4, 0)]</t>
-        </is>
-      </c>
-      <c r="E153" t="inlineStr"/>
-      <c r="F153" t="n">
-        <v>8.999999999999982</v>
-      </c>
-      <c r="G153" t="n">
-        <v>59.69999999999999</v>
-      </c>
-      <c r="H153" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="1" t="inlineStr">
-        <is>
-          <t>((13, 1), 3)</t>
-        </is>
-      </c>
-      <c r="B154" t="n">
-        <v>39.37</v>
-      </c>
-      <c r="C154" t="inlineStr"/>
-      <c r="D154" t="inlineStr"/>
-      <c r="E154" t="inlineStr"/>
-      <c r="F154" t="n">
-        <v>0</v>
-      </c>
-      <c r="G154" t="n">
-        <v>0</v>
-      </c>
-      <c r="H154" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="inlineStr">
-        <is>
-          <t>((13, 1), 4)</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr"/>
-      <c r="C155" t="inlineStr"/>
-      <c r="D155" t="inlineStr"/>
-      <c r="E155" t="inlineStr"/>
-      <c r="F155" t="n">
-        <v>0</v>
-      </c>
-      <c r="G155" t="n">
-        <v>0</v>
-      </c>
-      <c r="H155" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="inlineStr">
-        <is>
-          <t>((13, 1), 5)</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr"/>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
-      <c r="F156" t="n">
-        <v>0</v>
-      </c>
-      <c r="G156" t="n">
-        <v>0</v>
-      </c>
-      <c r="H156" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="inlineStr">
-        <is>
-          <t>((13, 2), 1)</t>
-        </is>
-      </c>
-      <c r="B157" t="n">
-        <v>46.6</v>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>[((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0), ((1, 3), 46.0, 0), ((1, 3), 46.2, 0), ((1, 3), 46.4, 0), ((1, 3), 46.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr"/>
-      <c r="E157" t="inlineStr"/>
-      <c r="F157" t="n">
-        <v>9.000000000000014</v>
-      </c>
-      <c r="G157" t="n">
-        <v>191.6999999999999</v>
-      </c>
-      <c r="H157" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="inlineStr">
-        <is>
-          <t>((13, 2), 2)</t>
-        </is>
-      </c>
-      <c r="B158" t="n">
-        <v>59.8</v>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>[((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0), ((1, 3), 46.0, 0), ((1, 3), 46.2, 0), ((1, 3), 46.4, 0), ((1, 3), 46.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>[((2, 3), 59.2, 0), ((2, 3), 59.4, 0), ((2, 3), 59.6, 0), ((2, 3), 59.8, 0)]</t>
-        </is>
-      </c>
-      <c r="E158" t="inlineStr"/>
-      <c r="F158" t="n">
-        <v>1.199999999999989</v>
-      </c>
-      <c r="G158" t="n">
-        <v>23.88</v>
-      </c>
-      <c r="H158" t="n">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="1" t="inlineStr">
-        <is>
-          <t>((13, 2), 3)</t>
-        </is>
-      </c>
-      <c r="B159" t="n">
-        <v>65.77</v>
-      </c>
-      <c r="C159" t="inlineStr"/>
-      <c r="D159" t="inlineStr"/>
-      <c r="E159" t="inlineStr"/>
-      <c r="F159" t="n">
-        <v>0</v>
-      </c>
-      <c r="G159" t="n">
-        <v>0</v>
-      </c>
-      <c r="H159" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="1" t="inlineStr">
-        <is>
-          <t>((13, 2), 4)</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
-      <c r="D160" t="inlineStr"/>
-      <c r="E160" t="inlineStr"/>
-      <c r="F160" t="n">
-        <v>0</v>
-      </c>
-      <c r="G160" t="n">
-        <v>0</v>
-      </c>
-      <c r="H160" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="1" t="inlineStr">
-        <is>
-          <t>((13, 2), 5)</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr"/>
-      <c r="D161" t="inlineStr"/>
-      <c r="E161" t="inlineStr"/>
-      <c r="F161" t="n">
-        <v>0</v>
-      </c>
-      <c r="G161" t="n">
-        <v>0</v>
-      </c>
-      <c r="H161" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="1" t="inlineStr">
-        <is>
-          <t>((14, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B162" t="n">
-        <v>40.6</v>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>[((1, 3), 40.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr"/>
-      <c r="E162" t="inlineStr"/>
-      <c r="F162" t="n">
-        <v>0</v>
-      </c>
-      <c r="G162" t="n">
-        <v>20.37</v>
-      </c>
-      <c r="H162" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="1" t="inlineStr">
-        <is>
-          <t>((14, 1), 2)</t>
-        </is>
-      </c>
-      <c r="B163" t="n">
-        <v>55</v>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>[((1, 3), 40.6, 0)]</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>[((2, 3), 51.4, 0), ((2, 3), 51.6, 0), ((2, 3), 51.8, 0), ((2, 3), 52.0, 0), ((2, 3), 52.2, 0), ((2, 3), 52.4, 0), ((2, 3), 52.6, 0), ((2, 3), 52.8, 0), ((2, 3), 53.0, 0), ((2, 3), 53.2, 0), ((2, 3), 53.4, 0), ((2, 3), 53.6, 0), ((2, 3), 53.8, 0), ((2, 3), 54.0, 0), ((2, 3), 54.2, 0), ((2, 3), 54.4, 0), ((2, 3), 54.6, 0), ((2, 3), 54.8, 0), ((2, 3), 55.0, 0)]</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr"/>
-      <c r="F163" t="n">
-        <v>34.2</v>
-      </c>
-      <c r="G163" t="n">
-        <v>113.43</v>
-      </c>
-      <c r="H163" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="1" t="inlineStr">
-        <is>
-          <t>((14, 1), 3)</t>
-        </is>
-      </c>
-      <c r="B164" t="n">
-        <v>60.97</v>
-      </c>
-      <c r="C164" t="inlineStr"/>
-      <c r="D164" t="inlineStr"/>
-      <c r="E164" t="inlineStr"/>
-      <c r="F164" t="n">
-        <v>0</v>
-      </c>
-      <c r="G164" t="n">
-        <v>0</v>
-      </c>
-      <c r="H164" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="1" t="inlineStr">
-        <is>
-          <t>((14, 1), 4)</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr"/>
-      <c r="C165" t="inlineStr"/>
-      <c r="D165" t="inlineStr"/>
-      <c r="E165" t="inlineStr"/>
-      <c r="F165" t="n">
-        <v>0</v>
-      </c>
-      <c r="G165" t="n">
-        <v>0</v>
-      </c>
-      <c r="H165" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="1" t="inlineStr">
-        <is>
-          <t>((14, 1), 5)</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr"/>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr"/>
-      <c r="F166" t="n">
-        <v>0</v>
-      </c>
-      <c r="G166" t="n">
-        <v>0</v>
-      </c>
-      <c r="H166" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="1" t="inlineStr">
-        <is>
-          <t>((15, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B167" t="n">
-        <v>50.8</v>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>[((1, 3), 50.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr"/>
-      <c r="E167" t="inlineStr"/>
-      <c r="F167" t="n">
-        <v>0</v>
-      </c>
-      <c r="G167" t="n">
-        <v>11.94</v>
-      </c>
-      <c r="H167" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="1" t="inlineStr">
-        <is>
-          <t>((15, 1), 2)</t>
-        </is>
-      </c>
-      <c r="B168" t="n">
-        <v>56.77</v>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>[((1, 3), 50.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr"/>
-      <c r="E168" t="inlineStr"/>
-      <c r="F168" t="n">
-        <v>0</v>
-      </c>
-      <c r="G168" t="n">
-        <v>0</v>
-      </c>
-      <c r="H168" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="1" t="inlineStr">
-        <is>
-          <t>((15, 1), 3)</t>
-        </is>
-      </c>
-      <c r="B169" t="n">
-        <v>62.74</v>
-      </c>
-      <c r="C169" t="inlineStr"/>
-      <c r="D169" t="inlineStr"/>
-      <c r="E169" t="inlineStr"/>
-      <c r="F169" t="n">
-        <v>0</v>
-      </c>
-      <c r="G169" t="n">
-        <v>0</v>
-      </c>
-      <c r="H169" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="1" t="inlineStr">
-        <is>
-          <t>((15, 1), 4)</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr"/>
-      <c r="C170" t="inlineStr"/>
-      <c r="D170" t="inlineStr"/>
-      <c r="E170" t="inlineStr"/>
-      <c r="F170" t="n">
-        <v>0</v>
-      </c>
-      <c r="G170" t="n">
-        <v>0</v>
-      </c>
-      <c r="H170" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="1" t="inlineStr">
-        <is>
-          <t>((15, 1), 5)</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr"/>
-      <c r="C171" t="inlineStr"/>
-      <c r="D171" t="inlineStr"/>
-      <c r="E171" t="inlineStr"/>
-      <c r="F171" t="n">
-        <v>0</v>
-      </c>
-      <c r="G171" t="n">
-        <v>0</v>
-      </c>
-      <c r="H171" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="1" t="inlineStr">
-        <is>
-          <t>((16, 1), 1)</t>
-        </is>
-      </c>
-      <c r="B172" t="n">
-        <v>52.8</v>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>[((1, 3), 51.0, 0), ((1, 3), 51.2, 0), ((1, 3), 51.4, 0), ((1, 3), 51.6, 0), ((1, 3), 51.8, 0), ((1, 3), 52.0, 0), ((1, 3), 52.2, 0), ((1, 3), 52.4, 0), ((1, 3), 52.6, 0), ((1, 3), 52.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr"/>
-      <c r="E172" t="inlineStr"/>
-      <c r="F172" t="n">
-        <v>8.999999999999972</v>
-      </c>
-      <c r="G172" t="n">
-        <v>119.4</v>
-      </c>
-      <c r="H172" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="1" t="inlineStr">
-        <is>
-          <t>((16, 1), 2)</t>
-        </is>
-      </c>
-      <c r="B173" t="n">
-        <v>58.77</v>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>[((1, 3), 51.0, 0), ((1, 3), 51.2, 0), ((1, 3), 51.4, 0), ((1, 3), 51.6, 0), ((1, 3), 51.8, 0), ((1, 3), 52.0, 0), ((1, 3), 52.2, 0), ((1, 3), 52.4, 0), ((1, 3), 52.6, 0), ((1, 3), 52.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr"/>
-      <c r="E173" t="inlineStr"/>
-      <c r="F173" t="n">
-        <v>0</v>
-      </c>
-      <c r="G173" t="n">
-        <v>0</v>
-      </c>
-      <c r="H173" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="1" t="inlineStr">
-        <is>
-          <t>((16, 1), 3)</t>
-        </is>
-      </c>
-      <c r="B174" t="n">
-        <v>64.73999999999999</v>
-      </c>
-      <c r="C174" t="inlineStr"/>
-      <c r="D174" t="inlineStr"/>
-      <c r="E174" t="inlineStr"/>
-      <c r="F174" t="n">
-        <v>0</v>
-      </c>
-      <c r="G174" t="n">
-        <v>0</v>
-      </c>
-      <c r="H174" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="1" t="inlineStr">
-        <is>
-          <t>((16, 1), 4)</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="inlineStr"/>
-      <c r="D175" t="inlineStr"/>
-      <c r="E175" t="inlineStr"/>
-      <c r="F175" t="n">
-        <v>0</v>
-      </c>
-      <c r="G175" t="n">
-        <v>0</v>
-      </c>
-      <c r="H175" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" s="1" t="inlineStr">
-        <is>
-          <t>((16, 1), 5)</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr"/>
-      <c r="C176" t="inlineStr"/>
-      <c r="D176" t="inlineStr"/>
-      <c r="E176" t="inlineStr"/>
-      <c r="F176" t="n">
-        <v>0</v>
-      </c>
-      <c r="G176" t="n">
-        <v>0</v>
-      </c>
-      <c r="H176" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
re-design initial solution build
</commit_message>
<xml_diff>
--- a/Exports/entire_solution.xlsx
+++ b/Exports/entire_solution.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.96</v>
+        <v>1.8</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -481,17 +481,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[((1, 2), 0.0, 0), ((1, 2), 7.96, 0)]</t>
+          <t>[((1, 2), 0.0, 0)]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>78.55999999999999</v>
+        <v>10.8</v>
       </c>
       <c r="F2" t="n">
-        <v>131.34</v>
+        <v>125.37</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="3">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13.93</v>
+        <v>7.77</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -526,26 +526,26 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.9</v>
+        <v>13.74</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[((3, 5), 0.0, 0), ((3, 5), 7.96, 0)]</t>
+          <t>[((3, 5), 0.0, 0)]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[((3, 4), 0.0, 0), ((3, 4), 7.96, 0)]</t>
+          <t>[((3, 4), 0.0, 0)]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>63.67999999999999</v>
+        <v>27.48</v>
       </c>
       <c r="F4" t="n">
-        <v>35.82000000000001</v>
+        <v>17.91</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
@@ -555,11 +555,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25.87</v>
+        <v>19.71</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[((3, 5), 0.0, 0), ((3, 5), 7.96, 0)]</t>
+          <t>[((3, 5), 0.0, 0)]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>31.84</v>
+        <v>25.68</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -601,26 +601,26 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>39.8</v>
+        <v>31.84</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[((1, 3), 4.0, 0), ((1, 3), 4.2, 0), ((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0)]</t>
+          <t>[((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0), ((1, 3), 6.0, 0), ((1, 3), 6.2, 0)]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[((1, 2), 31.84, 0), ((1, 2), 39.8, 0)]</t>
+          <t>[((1, 2), 31.84, 0)]</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>356.9599999999999</v>
+        <v>265.4</v>
       </c>
       <c r="F7" t="n">
-        <v>131.34</v>
+        <v>125.37</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="8">
@@ -630,11 +630,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>45.77</v>
+        <v>37.81</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[((1, 3), 4.0, 0), ((1, 3), 4.2, 0), ((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0)]</t>
+          <t>[((1, 3), 4.4, 0), ((1, 3), 4.6, 0), ((1, 3), 4.8, 0), ((1, 3), 5.0, 0), ((1, 3), 5.2, 0), ((1, 3), 5.4, 0), ((1, 3), 5.6, 0), ((1, 3), 5.8, 0), ((1, 3), 6.0, 0), ((1, 3), 6.2, 0)]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -655,26 +655,26 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>51.74</v>
+        <v>43.78</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[((3, 5), 31.84, 0), ((3, 5), 39.8, 0)]</t>
+          <t>[((3, 5), 31.84, 0)]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[((3, 4), 31.84, 0), ((3, 4), 39.8, 0)]</t>
+          <t>[((3, 4), 31.84, 0)]</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>63.68000000000001</v>
+        <v>23.88</v>
       </c>
       <c r="F9" t="n">
-        <v>35.81999999999999</v>
+        <v>17.91</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10">
@@ -684,11 +684,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>57.71</v>
+        <v>49.75</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[((3, 5), 31.84, 0), ((3, 5), 39.8, 0)]</t>
+          <t>[((3, 5), 31.84, 0)]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>63.68</v>
+        <v>55.72</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -730,26 +730,26 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23.88</v>
+        <v>7.96</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[((1, 3), 2.0, 0), ((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0)]</t>
+          <t>[((1, 3), 2.0, 0)]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[((1, 2), 15.92, 0), ((1, 2), 23.88, 0)]</t>
+          <t>[((1, 2), 7.96, 0)]</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>217.76</v>
+        <v>5.96</v>
       </c>
       <c r="F12" t="n">
-        <v>131.34</v>
+        <v>17.91</v>
       </c>
       <c r="G12" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13">
@@ -759,11 +759,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>29.85</v>
+        <v>13.93</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[((1, 3), 2.0, 0), ((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0)]</t>
+          <t>[((1, 3), 2.0, 0)]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -774,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14">
@@ -784,26 +784,26 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>35.82</v>
+        <v>19.9</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[((3, 5), 15.92, 0), ((3, 5), 23.88, 0)]</t>
+          <t>[((3, 5), 7.96, 0)]</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[((3, 4), 15.92, 0), ((3, 4), 23.88, 0)]</t>
+          <t>[((3, 4), 7.96, 0)]</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>63.67999999999999</v>
+        <v>23.88</v>
       </c>
       <c r="F14" t="n">
-        <v>35.81999999999999</v>
+        <v>17.91</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15">
@@ -813,11 +813,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>41.79</v>
+        <v>25.87</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[((3, 5), 15.92, 0), ((3, 5), 23.88, 0)]</t>
+          <t>[((3, 5), 7.96, 0)]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16">
@@ -838,7 +838,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47.76</v>
+        <v>31.84</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
@@ -859,26 +859,26 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>55.72</v>
+        <v>39.8</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[((1, 3), 6.0, 0), ((1, 3), 6.2, 0), ((1, 3), 6.4, 0), ((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0)]</t>
+          <t>[((1, 3), 6.4, 0)]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[((1, 2), 47.76, 0), ((1, 2), 55.72, 0)]</t>
+          <t>[((1, 2), 39.8, 0)]</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>496.16</v>
+        <v>33.4</v>
       </c>
       <c r="F17" t="n">
-        <v>131.34</v>
+        <v>17.91000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18">
@@ -888,11 +888,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>61.69</v>
+        <v>45.77</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[((1, 3), 6.0, 0), ((1, 3), 6.2, 0), ((1, 3), 6.4, 0), ((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0)]</t>
+          <t>[((1, 3), 6.4, 0)]</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19">
@@ -913,26 +913,26 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>67.66</v>
+        <v>51.74</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[((3, 5), 47.76, 0), ((3, 5), 55.72, 0)]</t>
+          <t>[((3, 5), 39.8, 0)]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[((3, 4), 47.76, 0), ((3, 4), 55.72, 0)]</t>
+          <t>[((3, 4), 39.8, 0)]</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>63.67999999999999</v>
+        <v>23.88000000000001</v>
       </c>
       <c r="F19" t="n">
-        <v>35.81999999999999</v>
+        <v>17.91</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
@@ -942,11 +942,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>73.63</v>
+        <v>57.71</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[((3, 5), 47.76, 0), ((3, 5), 55.72, 0)]</t>
+          <t>[((3, 5), 39.8, 0)]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21">
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>79.59999999999999</v>
+        <v>63.68</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
@@ -987,17 +987,27 @@
           <t>((3, 1), 1)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="B22" t="n">
+        <v>15.92</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>[((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0), ((1, 3), 4.0, 0)]</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>[((1, 2), 15.92, 0)]</t>
+        </is>
+      </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>128.2</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>125.37</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="23">
@@ -1006,8 +1016,14 @@
           <t>((3, 1), 2)</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
+      <c r="B23" t="n">
+        <v>21.89</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>[((1, 3), 2.2, 0), ((1, 3), 2.4, 0), ((1, 3), 2.6, 0), ((1, 3), 2.8, 0), ((1, 3), 3.0, 0), ((1, 3), 3.2, 0), ((1, 3), 3.4, 0), ((1, 3), 3.6, 0), ((1, 3), 3.8, 0), ((1, 3), 4.0, 0)]</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>0</v>
@@ -1016,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24">
@@ -1025,17 +1041,27 @@
           <t>((3, 1), 3)</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="B24" t="n">
+        <v>27.86</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>[((3, 5), 15.92, 0)]</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>[((3, 4), 15.92, 0)]</t>
+        </is>
+      </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>23.88</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>17.91</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25">
@@ -1045,11 +1071,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>33.83</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[((4, 5), 0.0, 0)]</t>
+          <t>[((3, 5), 15.92, 0)]</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -1057,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>5.97</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
         <v>0.05</v>
@@ -1070,7 +1096,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5.97</v>
+        <v>39.8</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
@@ -1090,17 +1116,27 @@
           <t>((3, 2), 1)</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="B27" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>[((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0), ((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0)]</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>[((1, 2), 47.76, 0)]</t>
+        </is>
+      </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>402.6</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>125.37</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="28">
@@ -1109,8 +1145,14 @@
           <t>((3, 2), 2)</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
+      <c r="B28" t="n">
+        <v>53.73</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>[((1, 3), 6.6, 0), ((1, 3), 6.8, 0), ((1, 3), 7.0, 0), ((1, 3), 7.2, 0), ((1, 3), 7.4, 0), ((1, 3), 7.6, 0), ((1, 3), 7.8, 0), ((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0)]</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
         <v>0</v>
@@ -1119,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29">
@@ -1128,7 +1170,9 @@
           <t>((3, 2), 3)</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="n">
+        <v>59.7</v>
+      </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
@@ -1147,23 +1191,17 @@
           <t>((3, 2), 4)</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>47.75</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>[((4, 5), 47.75, 0)]</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>5.969999999999999</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1172,9 +1210,7 @@
           <t>((3, 2), 5)</t>
         </is>
       </c>
-      <c r="B31" t="n">
-        <v>53.72</v>
-      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
@@ -1190,86 +1226,100 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 1)</t>
+          <t>((4, 1), 1)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>54.8</v>
+        <v>23.88</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[((1, 3), 53.0, 0), ((1, 3), 53.2, 0), ((1, 3), 53.4, 0), ((1, 3), 53.6, 0), ((1, 3), 53.8, 0), ((1, 3), 54.0, 0), ((1, 3), 54.2, 0), ((1, 3), 54.4, 0), ((1, 3), 54.6, 0), ((1, 3), 54.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
+          <t>[((1, 3), 4.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>[((1, 2), 23.88, 0)]</t>
+        </is>
+      </c>
       <c r="E32" t="n">
-        <v>8.999999999999972</v>
+        <v>19.68</v>
       </c>
       <c r="F32" t="n">
-        <v>119.4</v>
+        <v>17.91</v>
       </c>
       <c r="G32" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 2)</t>
+          <t>((4, 1), 2)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>60.77</v>
+        <v>29.85</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[((1, 3), 53.0, 0), ((1, 3), 53.2, 0), ((1, 3), 53.4, 0), ((1, 3), 53.6, 0), ((1, 3), 53.8, 0), ((1, 3), 54.0, 0), ((1, 3), 54.2, 0), ((1, 3), 54.4, 0), ((1, 3), 54.6, 0), ((1, 3), 54.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>[((2, 3), 53.0, 0), ((2, 3), 53.2, 0), ((2, 3), 53.4, 0), ((2, 3), 53.6, 0), ((2, 3), 53.8, 0), ((2, 3), 54.0, 0), ((2, 3), 54.2, 0), ((2, 3), 54.4, 0), ((2, 3), 54.6, 0), ((2, 3), 54.8, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 4.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>68.70000000000003</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>59.69999999999992</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 3)</t>
+          <t>((4, 1), 3)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>66.73999999999999</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+        <v>35.82</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>[((3, 5), 23.88, 0)]</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>[((3, 4), 23.88, 0)]</t>
+        </is>
+      </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>23.88</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>17.91</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 4)</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
+          <t>((4, 1), 4)</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>41.79</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>[((3, 5), 23.88, 0)]</t>
+        </is>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
         <v>0</v>
@@ -1278,16 +1328,18 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>((3, 3), 5)</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr"/>
+          <t>((4, 1), 5)</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>47.76</v>
+      </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
@@ -1303,65 +1355,65 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 1)</t>
+          <t>((4, 2), 1)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>9.800000000000001</v>
+        <v>55.72</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0), ((1, 3), 8.6, 0), ((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr"/>
+          <t>[((1, 3), 8.6, 0)]</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>[((1, 2), 55.72, 0)]</t>
+        </is>
+      </c>
       <c r="E37" t="n">
-        <v>9.000000000000007</v>
+        <v>47.12</v>
       </c>
       <c r="F37" t="n">
-        <v>119.4</v>
+        <v>17.91</v>
       </c>
       <c r="G37" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 2)</t>
+          <t>((4, 2), 2)</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>15.77</v>
+        <v>61.69</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[((1, 3), 8.0, 0), ((1, 3), 8.2, 0), ((1, 3), 8.4, 0), ((1, 3), 8.6, 0), ((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0)]</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>[((2, 3), 0.0, 0), ((2, 3), 0.2, 0), ((2, 3), 0.4, 0), ((2, 3), 0.6, 0), ((2, 3), 0.8, 0), ((2, 3), 1.0, 0), ((2, 3), 1.2, 0), ((2, 3), 1.4, 0), ((2, 3), 1.6, 0), ((2, 3), 1.8, 0)]</t>
-        </is>
-      </c>
+          <t>[((1, 3), 8.6, 0)]</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>148.7</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>59.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 3)</t>
+          <t>((4, 2), 3)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>21.74</v>
+        <v>67.66</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
@@ -1378,7 +1430,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 4)</t>
+          <t>((4, 2), 4)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1397,7 +1449,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>((4, 1), 5)</t>
+          <t>((4, 2), 5)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1416,20 +1468,20 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 1)</t>
+          <t>((5, 1), 1)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>28.2</v>
+        <v>10.6</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
+          <t>[((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0), ((1, 3), 10.0, 0), ((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0)]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>8.999999999999993</v>
+        <v>8.999999999999996</v>
       </c>
       <c r="F42" t="n">
         <v>119.4</v>
@@ -1441,24 +1493,24 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 2)</t>
+          <t>((5, 1), 2)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>34.17</v>
+        <v>16.57</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
+          <t>[((1, 3), 8.8, 0), ((1, 3), 9.0, 0), ((1, 3), 9.2, 0), ((1, 3), 9.4, 0), ((1, 3), 9.6, 0), ((1, 3), 9.8, 0), ((1, 3), 10.0, 0), ((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0)]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[((2, 3), 22.4, 0), ((2, 3), 22.6, 0), ((2, 3), 22.8, 0), ((2, 3), 23.0, 0), ((2, 3), 23.2, 0), ((2, 3), 23.4, 0), ((2, 3), 23.6, 0), ((2, 3), 23.8, 0), ((2, 3), 24.0, 0), ((2, 3), 24.2, 0)]</t>
+          <t>[((2, 3), 0.0, 0), ((2, 3), 0.2, 0), ((2, 3), 0.4, 0), ((2, 3), 0.6, 0), ((2, 3), 0.8, 0), ((2, 3), 1.0, 0), ((2, 3), 1.2, 0), ((2, 3), 1.4, 0), ((2, 3), 1.6, 0), ((2, 3), 1.8, 0)]</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>108.7</v>
+        <v>156.7</v>
       </c>
       <c r="F43" t="n">
         <v>59.69999999999999</v>
@@ -1470,11 +1522,11 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 3)</t>
+          <t>((5, 1), 3)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>40.14</v>
+        <v>22.54</v>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
@@ -1491,7 +1543,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 4)</t>
+          <t>((5, 1), 4)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1510,7 +1562,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>((4, 2), 5)</t>
+          <t>((5, 1), 5)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1529,20 +1581,20 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 1)</t>
+          <t>((5, 2), 1)</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>46.6</v>
+        <v>30.4</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0), ((1, 3), 46.0, 0), ((1, 3), 46.2, 0), ((1, 3), 46.4, 0), ((1, 3), 46.6, 0)]</t>
+          <t>[((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0), ((1, 3), 30.4, 0)]</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>9.000000000000014</v>
+        <v>8.999999999999986</v>
       </c>
       <c r="F47" t="n">
         <v>119.4</v>
@@ -1554,27 +1606,27 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 2)</t>
+          <t>((5, 2), 2)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>52.57</v>
+        <v>36.37</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0), ((1, 3), 46.0, 0), ((1, 3), 46.2, 0), ((1, 3), 46.4, 0), ((1, 3), 46.6, 0)]</t>
+          <t>[((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0), ((1, 3), 30.4, 0)]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[((2, 3), 44.8, 0), ((2, 3), 45.0, 0), ((2, 3), 45.2, 0), ((2, 3), 45.4, 0), ((2, 3), 45.6, 0), ((2, 3), 45.8, 0), ((2, 3), 46.0, 0), ((2, 3), 46.2, 0), ((2, 3), 46.4, 0), ((2, 3), 46.6, 0)]</t>
+          <t>[((2, 3), 19.8, 0), ((2, 3), 20.0, 0), ((2, 3), 20.2, 0), ((2, 3), 20.4, 0), ((2, 3), 20.6, 0), ((2, 3), 20.8, 0), ((2, 3), 21.0, 0), ((2, 3), 21.2, 0), ((2, 3), 21.4, 0), ((2, 3), 21.6, 0)]</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>68.7</v>
+        <v>156.7</v>
       </c>
       <c r="F48" t="n">
-        <v>59.69999999999999</v>
+        <v>59.70000000000006</v>
       </c>
       <c r="G48" t="n">
         <v>1</v>
@@ -1583,11 +1635,11 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 3)</t>
+          <t>((5, 2), 3)</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>58.54</v>
+        <v>42.34</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
@@ -1604,7 +1656,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 4)</t>
+          <t>((5, 2), 4)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1623,7 +1675,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>((4, 3), 5)</t>
+          <t>((5, 2), 5)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1642,15 +1694,15 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 1)</t>
+          <t>((6, 1), 1)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10</v>
+        <v>10.8</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.0, 0)]</t>
+          <t>[((1, 3), 10.8, 0)]</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
@@ -1667,40 +1719,40 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 2)</t>
+          <t>((6, 1), 2)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>15.97</v>
+        <v>16.77</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.0, 0)]</t>
+          <t>[((1, 3), 10.8, 0)]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[((2, 3), 2.0, 0), ((2, 3), 2.2, 0), ((2, 3), 2.4, 0), ((2, 3), 2.6, 0), ((2, 3), 2.8, 0), ((2, 3), 3.0, 0), ((2, 3), 3.2, 0), ((2, 3), 3.4, 0), ((2, 3), 3.6, 0), ((2, 3), 3.8, 0), ((2, 3), 4.0, 0), ((2, 3), 4.2, 0), ((2, 3), 4.4, 0), ((2, 3), 4.6, 0), ((2, 3), 4.8, 0), ((2, 3), 5.0, 0), ((2, 3), 5.2, 0), ((2, 3), 5.4, 0), ((2, 3), 5.6, 0)]</t>
+          <t>[((2, 3), 2.0, 0)]</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>231.23</v>
+        <v>14.77</v>
       </c>
       <c r="F53" t="n">
-        <v>113.43</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 3)</t>
+          <t>((6, 1), 3)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>21.94</v>
+        <v>22.74</v>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
@@ -1717,7 +1769,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 4)</t>
+          <t>((6, 1), 4)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1736,7 +1788,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>((5, 1), 5)</t>
+          <t>((6, 1), 5)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1755,65 +1807,65 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 1)</t>
+          <t>((6, 2), 1)</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>30.2</v>
+        <v>30.6</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[((1, 3), 28.4, 0), ((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0)]</t>
+          <t>[((1, 3), 30.6, 0)]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>8.999999999999993</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G57" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 2)</t>
+          <t>((6, 2), 2)</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>36.17</v>
+        <v>36.57</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[((1, 3), 28.4, 0), ((1, 3), 28.6, 0), ((1, 3), 28.8, 0), ((1, 3), 29.0, 0), ((1, 3), 29.2, 0), ((1, 3), 29.4, 0), ((1, 3), 29.6, 0), ((1, 3), 29.8, 0), ((1, 3), 30.0, 0), ((1, 3), 30.2, 0)]</t>
+          <t>[((1, 3), 30.6, 0)]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[((2, 3), 24.4, 0), ((2, 3), 24.6, 0), ((2, 3), 24.8, 0), ((2, 3), 25.0, 0), ((2, 3), 25.2, 0), ((2, 3), 25.4, 0), ((2, 3), 25.6, 0), ((2, 3), 25.8, 0), ((2, 3), 26.0, 0), ((2, 3), 26.2, 0)]</t>
+          <t>[((2, 3), 21.8, 0)]</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>108.7</v>
+        <v>14.77</v>
       </c>
       <c r="F58" t="n">
-        <v>59.69999999999999</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 3)</t>
+          <t>((6, 2), 3)</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>42.14</v>
+        <v>42.54</v>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
@@ -1830,7 +1882,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 4)</t>
+          <t>((6, 2), 4)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1849,7 +1901,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>((5, 2), 5)</t>
+          <t>((6, 2), 5)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1868,20 +1920,20 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 1)</t>
+          <t>((7, 1), 1)</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>48.6</v>
+        <v>12.8</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[((1, 3), 46.8, 0), ((1, 3), 47.0, 0), ((1, 3), 47.2, 0), ((1, 3), 47.4, 0), ((1, 3), 47.6, 0), ((1, 3), 47.8, 0), ((1, 3), 48.0, 0), ((1, 3), 48.2, 0), ((1, 3), 48.4, 0), ((1, 3), 48.6, 0)]</t>
+          <t>[((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0), ((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0)]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>9.000000000000014</v>
+        <v>9.000000000000007</v>
       </c>
       <c r="F62" t="n">
         <v>119.4</v>
@@ -1893,24 +1945,24 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 2)</t>
+          <t>((7, 1), 2)</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>54.57</v>
+        <v>18.77</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[((1, 3), 46.8, 0), ((1, 3), 47.0, 0), ((1, 3), 47.2, 0), ((1, 3), 47.4, 0), ((1, 3), 47.6, 0), ((1, 3), 47.8, 0), ((1, 3), 48.0, 0), ((1, 3), 48.2, 0), ((1, 3), 48.4, 0), ((1, 3), 48.6, 0)]</t>
+          <t>[((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0), ((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0)]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>[((2, 3), 46.8, 0), ((2, 3), 47.0, 0), ((2, 3), 47.2, 0), ((2, 3), 47.4, 0), ((2, 3), 47.6, 0), ((2, 3), 47.8, 0), ((2, 3), 48.0, 0), ((2, 3), 48.2, 0), ((2, 3), 48.4, 0), ((2, 3), 48.6, 0)]</t>
+          <t>[((2, 3), 2.2, 0), ((2, 3), 2.4, 0), ((2, 3), 2.6, 0), ((2, 3), 2.8, 0), ((2, 3), 3.0, 0), ((2, 3), 3.2, 0), ((2, 3), 3.4, 0), ((2, 3), 3.6, 0), ((2, 3), 3.8, 0), ((2, 3), 4.0, 0)]</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>68.7</v>
+        <v>156.7</v>
       </c>
       <c r="F63" t="n">
         <v>59.69999999999999</v>
@@ -1922,11 +1974,11 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 3)</t>
+          <t>((7, 1), 3)</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>60.54</v>
+        <v>24.74</v>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
@@ -1943,7 +1995,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 4)</t>
+          <t>((7, 1), 4)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1962,7 +2014,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>((5, 3), 5)</t>
+          <t>((7, 1), 5)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1981,20 +2033,20 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 1)</t>
+          <t>((7, 2), 1)</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>12</v>
+        <v>32.6</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0), ((1, 3), 10.8, 0), ((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0)]</t>
+          <t>[((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0), ((1, 3), 32.6, 0)]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>9.000000000000011</v>
       </c>
       <c r="F67" t="n">
         <v>119.4</v>
@@ -2006,27 +2058,27 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 2)</t>
+          <t>((7, 2), 2)</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>17.97</v>
+        <v>38.57</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[((1, 3), 10.2, 0), ((1, 3), 10.4, 0), ((1, 3), 10.6, 0), ((1, 3), 10.8, 0), ((1, 3), 11.0, 0), ((1, 3), 11.2, 0), ((1, 3), 11.4, 0), ((1, 3), 11.6, 0), ((1, 3), 11.8, 0), ((1, 3), 12.0, 0)]</t>
+          <t>[((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0), ((1, 3), 32.6, 0)]</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>[((2, 3), 5.8, 0), ((2, 3), 6.0, 0), ((2, 3), 6.2, 0), ((2, 3), 6.4, 0), ((2, 3), 6.6, 0), ((2, 3), 6.8, 0), ((2, 3), 7.0, 0), ((2, 3), 7.2, 0), ((2, 3), 7.4, 0), ((2, 3), 7.6, 0)]</t>
+          <t>[((2, 3), 22.0, 0), ((2, 3), 22.2, 0), ((2, 3), 22.4, 0), ((2, 3), 22.6, 0), ((2, 3), 22.8, 0), ((2, 3), 23.0, 0), ((2, 3), 23.2, 0), ((2, 3), 23.4, 0), ((2, 3), 23.6, 0), ((2, 3), 23.8, 0)]</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>112.7</v>
+        <v>156.7</v>
       </c>
       <c r="F68" t="n">
-        <v>59.70000000000002</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G68" t="n">
         <v>1</v>
@@ -2035,11 +2087,11 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 3)</t>
+          <t>((7, 2), 3)</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>23.94</v>
+        <v>44.54</v>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
@@ -2056,7 +2108,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 4)</t>
+          <t>((7, 2), 4)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2075,7 +2127,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>((6, 1), 5)</t>
+          <t>((7, 2), 5)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2094,15 +2146,15 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 1)</t>
+          <t>((8, 1), 1)</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>30.4</v>
+        <v>13</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.4, 0)]</t>
+          <t>[((1, 3), 13.0, 0)]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -2119,40 +2171,40 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 2)</t>
+          <t>((8, 1), 2)</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>36.37</v>
+        <v>18.97</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.4, 0)]</t>
+          <t>[((1, 3), 13.0, 0)]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[((2, 3), 26.4, 0), ((2, 3), 26.6, 0), ((2, 3), 26.8, 0), ((2, 3), 27.0, 0), ((2, 3), 27.2, 0), ((2, 3), 27.4, 0), ((2, 3), 27.6, 0), ((2, 3), 27.8, 0), ((2, 3), 28.0, 0), ((2, 3), 28.2, 0), ((2, 3), 28.4, 0), ((2, 3), 28.6, 0), ((2, 3), 28.8, 0), ((2, 3), 29.0, 0), ((2, 3), 29.2, 0), ((2, 3), 29.4, 0), ((2, 3), 29.6, 0), ((2, 3), 29.8, 0), ((2, 3), 30.0, 0)]</t>
+          <t>[((2, 3), 4.2, 0)]</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>155.23</v>
+        <v>14.77</v>
       </c>
       <c r="F73" t="n">
-        <v>113.4300000000001</v>
+        <v>5.970000000000002</v>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 3)</t>
+          <t>((8, 1), 3)</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>42.34</v>
+        <v>24.94</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
@@ -2169,7 +2221,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 4)</t>
+          <t>((8, 1), 4)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2188,7 +2240,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>((6, 2), 5)</t>
+          <t>((8, 1), 5)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2207,65 +2259,65 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 1)</t>
+          <t>((8, 2), 1)</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>50.6</v>
+        <v>32.8</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[((1, 3), 48.8, 0), ((1, 3), 49.0, 0), ((1, 3), 49.2, 0), ((1, 3), 49.4, 0), ((1, 3), 49.6, 0), ((1, 3), 49.8, 0), ((1, 3), 50.0, 0), ((1, 3), 50.2, 0), ((1, 3), 50.4, 0), ((1, 3), 50.6, 0)]</t>
+          <t>[((1, 3), 32.8, 0)]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>9.000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G77" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 2)</t>
+          <t>((8, 2), 2)</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>56.57</v>
+        <v>38.77</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>[((1, 3), 48.8, 0), ((1, 3), 49.0, 0), ((1, 3), 49.2, 0), ((1, 3), 49.4, 0), ((1, 3), 49.6, 0), ((1, 3), 49.8, 0), ((1, 3), 50.0, 0), ((1, 3), 50.2, 0), ((1, 3), 50.4, 0), ((1, 3), 50.6, 0)]</t>
+          <t>[((1, 3), 32.8, 0)]</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>[((2, 3), 48.8, 0), ((2, 3), 49.0, 0), ((2, 3), 49.2, 0), ((2, 3), 49.4, 0), ((2, 3), 49.6, 0), ((2, 3), 49.8, 0), ((2, 3), 50.0, 0), ((2, 3), 50.2, 0), ((2, 3), 50.4, 0), ((2, 3), 50.6, 0)]</t>
+          <t>[((2, 3), 24.0, 0)]</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>68.7</v>
+        <v>14.77</v>
       </c>
       <c r="F78" t="n">
-        <v>59.69999999999999</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G78" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 3)</t>
+          <t>((8, 2), 3)</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>62.54</v>
+        <v>44.74</v>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
@@ -2282,7 +2334,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 4)</t>
+          <t>((8, 2), 4)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -2301,7 +2353,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>((6, 3), 5)</t>
+          <t>((8, 2), 5)</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -2320,15 +2372,15 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 1)</t>
+          <t>((9, 1), 1)</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>[((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0), ((1, 3), 13.0, 0), ((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0)]</t>
+          <t>[((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0), ((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0)]</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
@@ -2345,24 +2397,24 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 2)</t>
+          <t>((9, 1), 2)</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>19.97</v>
+        <v>20.97</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>[((1, 3), 12.2, 0), ((1, 3), 12.4, 0), ((1, 3), 12.6, 0), ((1, 3), 12.8, 0), ((1, 3), 13.0, 0), ((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0)]</t>
+          <t>[((1, 3), 13.2, 0), ((1, 3), 13.4, 0), ((1, 3), 13.6, 0), ((1, 3), 13.8, 0), ((1, 3), 14.0, 0), ((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0)]</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>[((2, 3), 7.8, 0), ((2, 3), 8.0, 0), ((2, 3), 8.2, 0), ((2, 3), 8.4, 0), ((2, 3), 8.6, 0), ((2, 3), 8.8, 0), ((2, 3), 9.0, 0), ((2, 3), 9.2, 0), ((2, 3), 9.4, 0), ((2, 3), 9.6, 0)]</t>
+          <t>[((2, 3), 4.4, 0), ((2, 3), 4.6, 0), ((2, 3), 4.8, 0), ((2, 3), 5.0, 0), ((2, 3), 5.2, 0), ((2, 3), 5.4, 0), ((2, 3), 5.6, 0), ((2, 3), 5.8, 0), ((2, 3), 6.0, 0), ((2, 3), 6.2, 0)]</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>112.7</v>
+        <v>156.7</v>
       </c>
       <c r="F83" t="n">
         <v>59.70000000000002</v>
@@ -2374,11 +2426,11 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 3)</t>
+          <t>((9, 1), 3)</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>25.94</v>
+        <v>26.94</v>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
@@ -2395,7 +2447,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 4)</t>
+          <t>((9, 1), 4)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2414,7 +2466,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>((7, 1), 5)</t>
+          <t>((9, 1), 5)</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2433,20 +2485,20 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 1)</t>
+          <t>((9, 2), 1)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>32.4</v>
+        <v>34.8</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.6, 0), ((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0)]</t>
+          <t>[((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0), ((1, 3), 34.6, 0), ((1, 3), 34.8, 0)]</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
-        <v>8.999999999999982</v>
+        <v>8.999999999999972</v>
       </c>
       <c r="F87" t="n">
         <v>119.4</v>
@@ -2458,40 +2510,40 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 2)</t>
+          <t>((9, 2), 2)</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>38.37</v>
+        <v>40.77</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>[((1, 3), 30.6, 0), ((1, 3), 30.8, 0), ((1, 3), 31.0, 0), ((1, 3), 31.2, 0), ((1, 3), 31.4, 0), ((1, 3), 31.6, 0), ((1, 3), 31.8, 0), ((1, 3), 32.0, 0), ((1, 3), 32.2, 0), ((1, 3), 32.4, 0)]</t>
+          <t>[((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0), ((1, 3), 34.6, 0), ((1, 3), 34.8, 0)]</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>[((2, 3), 30.2, 0), ((2, 3), 30.4, 0)]</t>
+          <t>[((2, 3), 24.2, 0), ((2, 3), 24.4, 0), ((2, 3), 24.6, 0), ((2, 3), 24.8, 0), ((2, 3), 25.0, 0), ((2, 3), 25.2, 0), ((2, 3), 25.4, 0), ((2, 3), 25.6, 0), ((2, 3), 25.8, 0), ((2, 3), 26.0, 0)]</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>16.14</v>
+        <v>156.7</v>
       </c>
       <c r="F88" t="n">
-        <v>11.94000000000001</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G88" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 3)</t>
+          <t>((9, 2), 3)</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>44.34</v>
+        <v>46.74</v>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
@@ -2508,7 +2560,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 4)</t>
+          <t>((9, 2), 4)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2527,7 +2579,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>((7, 2), 5)</t>
+          <t>((9, 2), 5)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2546,15 +2598,15 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>((7, 3), 1)</t>
+          <t>((10, 1), 1)</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>50.8</v>
+        <v>15.2</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>[((1, 3), 50.8, 0)]</t>
+          <t>[((1, 3), 15.2, 0)]</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
@@ -2571,24 +2623,24 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>((7, 3), 2)</t>
+          <t>((10, 1), 2)</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>56.77</v>
+        <v>21.17</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>[((1, 3), 50.8, 0)]</t>
+          <t>[((1, 3), 15.2, 0)]</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>[((2, 3), 50.8, 0)]</t>
+          <t>[((2, 3), 6.4, 0)]</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>5.970000000000006</v>
+        <v>14.77</v>
       </c>
       <c r="F93" t="n">
         <v>5.969999999999999</v>
@@ -2600,11 +2652,11 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>((7, 3), 3)</t>
+          <t>((10, 1), 3)</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>62.74</v>
+        <v>27.14</v>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
@@ -2621,7 +2673,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>((7, 3), 4)</t>
+          <t>((10, 1), 4)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2640,7 +2692,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>((7, 3), 5)</t>
+          <t>((10, 1), 5)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2659,65 +2711,65 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 1)</t>
+          <t>((10, 2), 1)</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>[((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0), ((1, 3), 15.2, 0), ((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0)]</t>
+          <t>[((1, 3), 35.0, 0)]</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G97" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 2)</t>
+          <t>((10, 2), 2)</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>21.97</v>
+        <v>40.97</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>[((1, 3), 14.2, 0), ((1, 3), 14.4, 0), ((1, 3), 14.6, 0), ((1, 3), 14.8, 0), ((1, 3), 15.0, 0), ((1, 3), 15.2, 0), ((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0)]</t>
+          <t>[((1, 3), 35.0, 0)]</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>[((2, 3), 9.8, 0), ((2, 3), 10.0, 0)]</t>
+          <t>[((2, 3), 26.2, 0)]</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>24.14</v>
+        <v>14.77</v>
       </c>
       <c r="F98" t="n">
-        <v>11.94</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G98" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 3)</t>
+          <t>((10, 2), 3)</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>27.94</v>
+        <v>46.94</v>
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
@@ -2734,7 +2786,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 4)</t>
+          <t>((10, 2), 4)</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -2753,7 +2805,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>((8, 1), 5)</t>
+          <t>((10, 2), 5)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2772,20 +2824,20 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 1)</t>
+          <t>((11, 1), 1)</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>34.4</v>
+        <v>17.2</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>[((1, 3), 32.6, 0), ((1, 3), 32.8, 0), ((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0)]</t>
+          <t>[((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0), ((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0)]</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="n">
-        <v>8.999999999999986</v>
+        <v>8.999999999999993</v>
       </c>
       <c r="F102" t="n">
         <v>119.4</v>
@@ -2797,27 +2849,27 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 2)</t>
+          <t>((11, 1), 2)</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>40.37</v>
+        <v>23.17</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>[((1, 3), 32.6, 0), ((1, 3), 32.8, 0), ((1, 3), 33.0, 0), ((1, 3), 33.2, 0), ((1, 3), 33.4, 0), ((1, 3), 33.6, 0), ((1, 3), 33.8, 0), ((1, 3), 34.0, 0), ((1, 3), 34.2, 0), ((1, 3), 34.4, 0)]</t>
+          <t>[((1, 3), 15.4, 0), ((1, 3), 15.6, 0), ((1, 3), 15.8, 0), ((1, 3), 16.0, 0), ((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0)]</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>[((2, 3), 30.6, 0), ((2, 3), 30.8, 0), ((2, 3), 31.0, 0), ((2, 3), 31.2, 0), ((2, 3), 31.4, 0), ((2, 3), 31.6, 0), ((2, 3), 31.8, 0), ((2, 3), 32.0, 0), ((2, 3), 32.2, 0), ((2, 3), 32.4, 0)]</t>
+          <t>[((2, 3), 6.6, 0), ((2, 3), 6.8, 0), ((2, 3), 7.0, 0), ((2, 3), 7.2, 0), ((2, 3), 7.4, 0), ((2, 3), 7.6, 0), ((2, 3), 7.8, 0), ((2, 3), 8.0, 0), ((2, 3), 8.2, 0), ((2, 3), 8.4, 0)]</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>88.69999999999996</v>
+        <v>156.7</v>
       </c>
       <c r="F103" t="n">
-        <v>59.70000000000006</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G103" t="n">
         <v>1</v>
@@ -2826,11 +2878,11 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 3)</t>
+          <t>((11, 1), 3)</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>46.34</v>
+        <v>29.14</v>
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
@@ -2847,7 +2899,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 4)</t>
+          <t>((11, 1), 4)</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2866,7 +2918,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>((8, 2), 5)</t>
+          <t>((11, 1), 5)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2885,20 +2937,20 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>((8, 3), 1)</t>
+          <t>((11, 2), 1)</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>52.8</v>
+        <v>37</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>[((1, 3), 51.0, 0), ((1, 3), 51.2, 0), ((1, 3), 51.4, 0), ((1, 3), 51.6, 0), ((1, 3), 51.8, 0), ((1, 3), 52.0, 0), ((1, 3), 52.2, 0), ((1, 3), 52.4, 0), ((1, 3), 52.6, 0), ((1, 3), 52.8, 0)]</t>
+          <t>[((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0), ((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0)]</t>
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="n">
-        <v>8.999999999999972</v>
+        <v>9</v>
       </c>
       <c r="F107" t="n">
         <v>119.4</v>
@@ -2910,27 +2962,27 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>((8, 3), 2)</t>
+          <t>((11, 2), 2)</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>58.77</v>
+        <v>42.97</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>[((1, 3), 51.0, 0), ((1, 3), 51.2, 0), ((1, 3), 51.4, 0), ((1, 3), 51.6, 0), ((1, 3), 51.8, 0), ((1, 3), 52.0, 0), ((1, 3), 52.2, 0), ((1, 3), 52.4, 0), ((1, 3), 52.6, 0), ((1, 3), 52.8, 0)]</t>
+          <t>[((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0), ((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0)]</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>[((2, 3), 51.0, 0), ((2, 3), 51.2, 0), ((2, 3), 51.4, 0), ((2, 3), 51.6, 0), ((2, 3), 51.8, 0), ((2, 3), 52.0, 0), ((2, 3), 52.2, 0), ((2, 3), 52.4, 0), ((2, 3), 52.6, 0), ((2, 3), 52.8, 0)]</t>
+          <t>[((2, 3), 26.4, 0), ((2, 3), 26.6, 0), ((2, 3), 26.8, 0), ((2, 3), 27.0, 0), ((2, 3), 27.2, 0), ((2, 3), 27.4, 0), ((2, 3), 27.6, 0), ((2, 3), 27.8, 0), ((2, 3), 28.0, 0), ((2, 3), 28.2, 0)]</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>68.70000000000003</v>
+        <v>156.7</v>
       </c>
       <c r="F108" t="n">
-        <v>59.69999999999992</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G108" t="n">
         <v>1</v>
@@ -2939,11 +2991,11 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>((8, 3), 3)</t>
+          <t>((11, 2), 3)</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>64.73999999999999</v>
+        <v>48.94</v>
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr"/>
@@ -2960,7 +3012,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>((8, 3), 4)</t>
+          <t>((11, 2), 4)</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -2979,7 +3031,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>((8, 3), 5)</t>
+          <t>((11, 2), 5)</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -2998,65 +3050,65 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 1)</t>
+          <t>((12, 1), 1)</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>18</v>
+        <v>17.4</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>[((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0), ((1, 3), 17.4, 0), ((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0)]</t>
+          <t>[((1, 3), 17.4, 0)]</t>
         </is>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G112" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 2)</t>
+          <t>((12, 1), 2)</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>23.97</v>
+        <v>23.37</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>[((1, 3), 16.2, 0), ((1, 3), 16.4, 0), ((1, 3), 16.6, 0), ((1, 3), 16.8, 0), ((1, 3), 17.0, 0), ((1, 3), 17.2, 0), ((1, 3), 17.4, 0), ((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0)]</t>
+          <t>[((1, 3), 17.4, 0)]</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>[((2, 3), 10.2, 0), ((2, 3), 10.4, 0), ((2, 3), 10.6, 0), ((2, 3), 10.8, 0), ((2, 3), 11.0, 0), ((2, 3), 11.2, 0), ((2, 3), 11.4, 0), ((2, 3), 11.6, 0), ((2, 3), 11.8, 0), ((2, 3), 12.0, 0)]</t>
+          <t>[((2, 3), 8.6, 0)]</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>128.7</v>
+        <v>14.77</v>
       </c>
       <c r="F113" t="n">
-        <v>59.70000000000002</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G113" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 3)</t>
+          <t>((12, 1), 3)</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>29.94</v>
+        <v>29.34</v>
       </c>
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
@@ -3073,7 +3125,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 4)</t>
+          <t>((12, 1), 4)</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -3092,7 +3144,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>((9, 1), 5)</t>
+          <t>((12, 1), 5)</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -3111,65 +3163,65 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 1)</t>
+          <t>((12, 2), 1)</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>36.4</v>
+        <v>37.2</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>[((1, 3), 34.6, 0), ((1, 3), 34.8, 0), ((1, 3), 35.0, 0), ((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0)]</t>
+          <t>[((1, 3), 37.2, 0)]</t>
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="n">
-        <v>8.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G117" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 2)</t>
+          <t>((12, 2), 2)</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>42.37</v>
+        <v>43.17</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>[((1, 3), 34.6, 0), ((1, 3), 34.8, 0), ((1, 3), 35.0, 0), ((1, 3), 35.2, 0), ((1, 3), 35.4, 0), ((1, 3), 35.6, 0), ((1, 3), 35.8, 0), ((1, 3), 36.0, 0), ((1, 3), 36.2, 0), ((1, 3), 36.4, 0)]</t>
+          <t>[((1, 3), 37.2, 0)]</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>[((2, 3), 32.6, 0), ((2, 3), 32.8, 0), ((2, 3), 33.0, 0), ((2, 3), 33.2, 0), ((2, 3), 33.4, 0), ((2, 3), 33.6, 0), ((2, 3), 33.8, 0), ((2, 3), 34.0, 0), ((2, 3), 34.2, 0), ((2, 3), 34.4, 0)]</t>
+          <t>[((2, 3), 28.4, 0)]</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>88.69999999999996</v>
+        <v>14.77</v>
       </c>
       <c r="F118" t="n">
-        <v>59.70000000000006</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G118" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 3)</t>
+          <t>((12, 2), 3)</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>48.34</v>
+        <v>49.14</v>
       </c>
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr"/>
@@ -3186,7 +3238,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 4)</t>
+          <t>((12, 2), 4)</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -3205,7 +3257,7 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>((9, 2), 5)</t>
+          <t>((12, 2), 5)</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -3224,20 +3276,20 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>((9, 3), 1)</t>
+          <t>((13, 1), 1)</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>56.8</v>
+        <v>19.4</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>[((1, 3), 55.0, 0), ((1, 3), 55.2, 0), ((1, 3), 55.4, 0), ((1, 3), 55.6, 0), ((1, 3), 55.8, 0), ((1, 3), 56.0, 0), ((1, 3), 56.2, 0), ((1, 3), 56.4, 0), ((1, 3), 56.6, 0), ((1, 3), 56.8, 0)]</t>
+          <t>[((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0), ((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0)]</t>
         </is>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="n">
-        <v>8.999999999999972</v>
+        <v>8.999999999999986</v>
       </c>
       <c r="F122" t="n">
         <v>119.4</v>
@@ -3249,27 +3301,27 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>((9, 3), 2)</t>
+          <t>((13, 1), 2)</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>62.77</v>
+        <v>25.37</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>[((1, 3), 55.0, 0), ((1, 3), 55.2, 0), ((1, 3), 55.4, 0), ((1, 3), 55.6, 0), ((1, 3), 55.8, 0), ((1, 3), 56.0, 0), ((1, 3), 56.2, 0), ((1, 3), 56.4, 0), ((1, 3), 56.6, 0), ((1, 3), 56.8, 0)]</t>
+          <t>[((1, 3), 17.6, 0), ((1, 3), 17.8, 0), ((1, 3), 18.0, 0), ((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0)]</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>[((2, 3), 55.0, 0), ((2, 3), 55.2, 0), ((2, 3), 55.4, 0), ((2, 3), 55.6, 0), ((2, 3), 55.8, 0), ((2, 3), 56.0, 0), ((2, 3), 56.2, 0), ((2, 3), 56.4, 0), ((2, 3), 56.6, 0), ((2, 3), 56.8, 0)]</t>
+          <t>[((2, 3), 8.8, 0), ((2, 3), 9.0, 0), ((2, 3), 9.2, 0), ((2, 3), 9.4, 0), ((2, 3), 9.6, 0), ((2, 3), 9.8, 0), ((2, 3), 10.0, 0), ((2, 3), 10.2, 0), ((2, 3), 10.4, 0), ((2, 3), 10.6, 0)]</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>68.70000000000003</v>
+        <v>156.7</v>
       </c>
       <c r="F123" t="n">
-        <v>59.69999999999992</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G123" t="n">
         <v>1</v>
@@ -3278,11 +3330,11 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>((9, 3), 3)</t>
+          <t>((13, 1), 3)</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>68.73999999999999</v>
+        <v>31.34</v>
       </c>
       <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr"/>
@@ -3299,7 +3351,7 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>((9, 3), 4)</t>
+          <t>((13, 1), 4)</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -3318,7 +3370,7 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>((9, 3), 5)</t>
+          <t>((13, 1), 5)</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -3337,20 +3389,20 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 1)</t>
+          <t>((13, 2), 1)</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>20</v>
+        <v>39.2</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>[((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0), ((1, 3), 19.6, 0), ((1, 3), 19.8, 0), ((1, 3), 20.0, 0)]</t>
+          <t>[((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0), ((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0)]</t>
         </is>
       </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="n">
-        <v>9</v>
+        <v>9.000000000000028</v>
       </c>
       <c r="F127" t="n">
         <v>119.4</v>
@@ -3362,27 +3414,27 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 2)</t>
+          <t>((13, 2), 2)</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>25.97</v>
+        <v>45.17</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>[((1, 3), 18.2, 0), ((1, 3), 18.4, 0), ((1, 3), 18.6, 0), ((1, 3), 18.8, 0), ((1, 3), 19.0, 0), ((1, 3), 19.2, 0), ((1, 3), 19.4, 0), ((1, 3), 19.6, 0), ((1, 3), 19.8, 0), ((1, 3), 20.0, 0)]</t>
+          <t>[((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0), ((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0)]</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>[((2, 3), 12.2, 0), ((2, 3), 12.4, 0), ((2, 3), 12.6, 0), ((2, 3), 12.8, 0), ((2, 3), 13.0, 0), ((2, 3), 13.2, 0), ((2, 3), 13.4, 0), ((2, 3), 13.6, 0), ((2, 3), 13.8, 0), ((2, 3), 14.0, 0)]</t>
+          <t>[((2, 3), 28.6, 0), ((2, 3), 28.8, 0), ((2, 3), 29.0, 0), ((2, 3), 29.2, 0), ((2, 3), 29.4, 0), ((2, 3), 29.6, 0), ((2, 3), 29.8, 0), ((2, 3), 30.0, 0), ((2, 3), 30.2, 0), ((2, 3), 30.4, 0)]</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>128.7</v>
+        <v>156.7</v>
       </c>
       <c r="F128" t="n">
-        <v>59.70000000000002</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G128" t="n">
         <v>1</v>
@@ -3391,11 +3443,11 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 3)</t>
+          <t>((13, 2), 3)</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>31.94</v>
+        <v>51.14</v>
       </c>
       <c r="C129" t="inlineStr"/>
       <c r="D129" t="inlineStr"/>
@@ -3412,7 +3464,7 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 4)</t>
+          <t>((13, 2), 4)</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -3431,7 +3483,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>((10, 1), 5)</t>
+          <t>((13, 2), 5)</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -3450,65 +3502,65 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 1)</t>
+          <t>((14, 1), 1)</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>38.4</v>
+        <v>19.6</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>[((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0), ((1, 3), 37.2, 0), ((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0)]</t>
+          <t>[((1, 3), 19.6, 0)]</t>
         </is>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="n">
-        <v>8.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G132" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 2)</t>
+          <t>((14, 1), 2)</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>44.37</v>
+        <v>25.57</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>[((1, 3), 36.6, 0), ((1, 3), 36.8, 0), ((1, 3), 37.0, 0), ((1, 3), 37.2, 0), ((1, 3), 37.4, 0), ((1, 3), 37.6, 0), ((1, 3), 37.8, 0), ((1, 3), 38.0, 0), ((1, 3), 38.2, 0), ((1, 3), 38.4, 0)]</t>
+          <t>[((1, 3), 19.6, 0)]</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>[((2, 3), 34.6, 0), ((2, 3), 34.8, 0), ((2, 3), 35.0, 0), ((2, 3), 35.2, 0), ((2, 3), 35.4, 0), ((2, 3), 35.6, 0), ((2, 3), 35.8, 0), ((2, 3), 36.0, 0), ((2, 3), 36.2, 0), ((2, 3), 36.4, 0)]</t>
+          <t>[((2, 3), 10.8, 0)]</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>88.69999999999996</v>
+        <v>14.77</v>
       </c>
       <c r="F133" t="n">
-        <v>59.70000000000006</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G133" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 3)</t>
+          <t>((14, 1), 3)</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>50.34</v>
+        <v>31.54</v>
       </c>
       <c r="C134" t="inlineStr"/>
       <c r="D134" t="inlineStr"/>
@@ -3525,7 +3577,7 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 4)</t>
+          <t>((14, 1), 4)</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
@@ -3544,7 +3596,7 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>((10, 2), 5)</t>
+          <t>((14, 1), 5)</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -3563,65 +3615,65 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>((10, 3), 1)</t>
+          <t>((14, 2), 1)</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>58.8</v>
+        <v>39.4</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>[((1, 3), 57.0, 0), ((1, 3), 57.2, 0), ((1, 3), 57.4, 0), ((1, 3), 57.6, 0), ((1, 3), 57.8, 0), ((1, 3), 58.0, 0), ((1, 3), 58.2, 0), ((1, 3), 58.4, 0), ((1, 3), 58.6, 0), ((1, 3), 58.8, 0)]</t>
+          <t>[((1, 3), 39.4, 0)]</t>
         </is>
       </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="n">
-        <v>8.999999999999972</v>
+        <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G137" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>((10, 3), 2)</t>
+          <t>((14, 2), 2)</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>64.77</v>
+        <v>45.37</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>[((1, 3), 57.0, 0), ((1, 3), 57.2, 0), ((1, 3), 57.4, 0), ((1, 3), 57.6, 0), ((1, 3), 57.8, 0), ((1, 3), 58.0, 0), ((1, 3), 58.2, 0), ((1, 3), 58.4, 0), ((1, 3), 58.6, 0), ((1, 3), 58.8, 0)]</t>
+          <t>[((1, 3), 39.4, 0)]</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>[((2, 3), 57.0, 0), ((2, 3), 57.2, 0), ((2, 3), 57.4, 0), ((2, 3), 57.6, 0), ((2, 3), 57.8, 0), ((2, 3), 58.0, 0), ((2, 3), 58.2, 0), ((2, 3), 58.4, 0), ((2, 3), 58.6, 0), ((2, 3), 58.8, 0)]</t>
+          <t>[((2, 3), 30.6, 0)]</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>68.69999999999996</v>
+        <v>14.77</v>
       </c>
       <c r="F138" t="n">
-        <v>59.69999999999999</v>
+        <v>5.970000000000006</v>
       </c>
       <c r="G138" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>((10, 3), 3)</t>
+          <t>((14, 2), 3)</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>70.73999999999999</v>
+        <v>51.34</v>
       </c>
       <c r="C139" t="inlineStr"/>
       <c r="D139" t="inlineStr"/>
@@ -3638,7 +3690,7 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>((10, 3), 4)</t>
+          <t>((14, 2), 4)</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -3657,7 +3709,7 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>((10, 3), 5)</t>
+          <t>((14, 2), 5)</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -3676,52 +3728,52 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 1)</t>
+          <t>((15, 1), 1)</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>20.2</v>
+        <v>21.6</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>[((1, 3), 20.2, 0)]</t>
+          <t>[((1, 3), 19.8, 0), ((1, 3), 20.0, 0), ((1, 3), 20.2, 0), ((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0)]</t>
         </is>
       </c>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="n">
-        <v>0</v>
+        <v>9.000000000000014</v>
       </c>
       <c r="F142" t="n">
-        <v>11.94</v>
+        <v>119.4</v>
       </c>
       <c r="G142" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 2)</t>
+          <t>((15, 1), 2)</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>26.17</v>
+        <v>27.57</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>[((1, 3), 20.2, 0)]</t>
+          <t>[((1, 3), 19.8, 0), ((1, 3), 20.0, 0), ((1, 3), 20.2, 0), ((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0)]</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>[((2, 3), 14.2, 0), ((2, 3), 14.4, 0), ((2, 3), 14.6, 0), ((2, 3), 14.8, 0), ((2, 3), 15.0, 0), ((2, 3), 15.2, 0), ((2, 3), 15.4, 0), ((2, 3), 15.6, 0), ((2, 3), 15.8, 0), ((2, 3), 16.0, 0), ((2, 3), 16.2, 0), ((2, 3), 16.4, 0), ((2, 3), 16.6, 0), ((2, 3), 16.8, 0), ((2, 3), 17.0, 0), ((2, 3), 17.2, 0), ((2, 3), 17.4, 0), ((2, 3), 17.6, 0), ((2, 3), 17.8, 0)]</t>
+          <t>[((2, 3), 11.0, 0), ((2, 3), 11.2, 0), ((2, 3), 11.4, 0), ((2, 3), 11.6, 0), ((2, 3), 11.8, 0), ((2, 3), 12.0, 0), ((2, 3), 12.2, 0), ((2, 3), 12.4, 0), ((2, 3), 12.6, 0), ((2, 3), 12.8, 0)]</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>193.23</v>
+        <v>156.7</v>
       </c>
       <c r="F143" t="n">
-        <v>113.43</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G143" t="n">
         <v>1</v>
@@ -3730,11 +3782,11 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 3)</t>
+          <t>((15, 1), 3)</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>32.14</v>
+        <v>33.54</v>
       </c>
       <c r="C144" t="inlineStr"/>
       <c r="D144" t="inlineStr"/>
@@ -3751,7 +3803,7 @@
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 4)</t>
+          <t>((15, 1), 4)</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -3770,7 +3822,7 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>((11, 1), 5)</t>
+          <t>((15, 1), 5)</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -3789,15 +3841,15 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 1)</t>
+          <t>((15, 2), 1)</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>40.4</v>
+        <v>41.4</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>[((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0), ((1, 3), 39.4, 0), ((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0)]</t>
+          <t>[((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0), ((1, 3), 40.6, 0), ((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0)]</t>
         </is>
       </c>
       <c r="D147" t="inlineStr"/>
@@ -3814,24 +3866,24 @@
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 2)</t>
+          <t>((15, 2), 2)</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>46.37</v>
+        <v>47.37</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>[((1, 3), 38.6, 0), ((1, 3), 38.8, 0), ((1, 3), 39.0, 0), ((1, 3), 39.2, 0), ((1, 3), 39.4, 0), ((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0)]</t>
+          <t>[((1, 3), 39.6, 0), ((1, 3), 39.8, 0), ((1, 3), 40.0, 0), ((1, 3), 40.2, 0), ((1, 3), 40.4, 0), ((1, 3), 40.6, 0), ((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0)]</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>[((2, 3), 36.6, 0), ((2, 3), 36.8, 0), ((2, 3), 37.0, 0), ((2, 3), 37.2, 0), ((2, 3), 37.4, 0), ((2, 3), 37.6, 0), ((2, 3), 37.8, 0), ((2, 3), 38.0, 0), ((2, 3), 38.2, 0), ((2, 3), 38.4, 0)]</t>
+          <t>[((2, 3), 30.8, 0), ((2, 3), 31.0, 0), ((2, 3), 31.2, 0), ((2, 3), 31.4, 0), ((2, 3), 31.6, 0), ((2, 3), 31.8, 0), ((2, 3), 32.0, 0), ((2, 3), 32.2, 0), ((2, 3), 32.4, 0), ((2, 3), 32.6, 0)]</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>88.69999999999996</v>
+        <v>156.7</v>
       </c>
       <c r="F148" t="n">
         <v>59.70000000000006</v>
@@ -3843,11 +3895,11 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 3)</t>
+          <t>((15, 2), 3)</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>52.34</v>
+        <v>53.34</v>
       </c>
       <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr"/>
@@ -3864,7 +3916,7 @@
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 4)</t>
+          <t>((15, 2), 4)</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
@@ -3883,7 +3935,7 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>((11, 2), 5)</t>
+          <t>((15, 2), 5)</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -3902,65 +3954,65 @@
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>((11, 3), 1)</t>
+          <t>((16, 1), 1)</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>59.8</v>
+        <v>21.8</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>[((1, 3), 59.0, 0), ((1, 3), 59.2, 0), ((1, 3), 59.4, 0), ((1, 3), 59.6, 0), ((1, 3), 59.8, 0)]</t>
+          <t>[((1, 3), 21.8, 0)]</t>
         </is>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="n">
-        <v>1.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>59.69999999999999</v>
+        <v>11.94</v>
       </c>
       <c r="G152" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>((11, 3), 2)</t>
+          <t>((16, 1), 2)</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>65.77</v>
+        <v>27.77</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>[((1, 3), 59.0, 0), ((1, 3), 59.2, 0), ((1, 3), 59.4, 0), ((1, 3), 59.6, 0), ((1, 3), 59.8, 0)]</t>
+          <t>[((1, 3), 21.8, 0)]</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>[((2, 3), 59.0, 0), ((2, 3), 59.2, 0), ((2, 3), 59.4, 0), ((2, 3), 59.6, 0), ((2, 3), 59.8, 0)]</t>
+          <t>[((2, 3), 13.0, 0)]</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>31.84999999999998</v>
+        <v>14.77</v>
       </c>
       <c r="F153" t="n">
-        <v>29.84999999999999</v>
+        <v>5.970000000000002</v>
       </c>
       <c r="G153" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>((11, 3), 3)</t>
+          <t>((16, 1), 3)</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>71.73999999999999</v>
+        <v>33.74</v>
       </c>
       <c r="C154" t="inlineStr"/>
       <c r="D154" t="inlineStr"/>
@@ -3977,7 +4029,7 @@
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>((11, 3), 4)</t>
+          <t>((16, 1), 4)</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
@@ -3996,7 +4048,7 @@
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>((11, 3), 5)</t>
+          <t>((16, 1), 5)</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -4015,65 +4067,65 @@
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 1)</t>
+          <t>((16, 2), 1)</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>22.2</v>
+        <v>41.6</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>[((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0), ((1, 3), 21.8, 0), ((1, 3), 22.0, 0), ((1, 3), 22.2, 0)]</t>
+          <t>[((1, 3), 41.6, 0)]</t>
         </is>
       </c>
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="n">
-        <v>8.999999999999993</v>
+        <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G157" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 2)</t>
+          <t>((16, 2), 2)</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>28.17</v>
+        <v>47.57</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>[((1, 3), 20.4, 0), ((1, 3), 20.6, 0), ((1, 3), 20.8, 0), ((1, 3), 21.0, 0), ((1, 3), 21.2, 0), ((1, 3), 21.4, 0), ((1, 3), 21.6, 0), ((1, 3), 21.8, 0), ((1, 3), 22.0, 0), ((1, 3), 22.2, 0)]</t>
+          <t>[((1, 3), 41.6, 0)]</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>[((2, 3), 18.0, 0), ((2, 3), 18.2, 0), ((2, 3), 18.4, 0), ((2, 3), 18.6, 0), ((2, 3), 18.8, 0), ((2, 3), 19.0, 0), ((2, 3), 19.2, 0), ((2, 3), 19.4, 0), ((2, 3), 19.6, 0), ((2, 3), 19.8, 0)]</t>
+          <t>[((2, 3), 32.8, 0)]</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>92.70000000000002</v>
+        <v>14.77</v>
       </c>
       <c r="F158" t="n">
-        <v>59.69999999999999</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G158" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 3)</t>
+          <t>((16, 2), 3)</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>34.14</v>
+        <v>53.54</v>
       </c>
       <c r="C159" t="inlineStr"/>
       <c r="D159" t="inlineStr"/>
@@ -4090,7 +4142,7 @@
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 4)</t>
+          <t>((16, 2), 4)</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
@@ -4109,7 +4161,7 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>((12, 1), 5)</t>
+          <t>((16, 2), 5)</t>
         </is>
       </c>
       <c r="B161" t="inlineStr"/>
@@ -4128,65 +4180,65 @@
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 1)</t>
+          <t>((17, 1), 1)</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>40.6</v>
+        <v>23.8</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>[((1, 3), 40.6, 0)]</t>
+          <t>[((1, 3), 22.0, 0), ((1, 3), 22.2, 0), ((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0)]</t>
         </is>
       </c>
       <c r="D162" t="inlineStr"/>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>9.000000000000007</v>
       </c>
       <c r="F162" t="n">
-        <v>11.94</v>
+        <v>119.4</v>
       </c>
       <c r="G162" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 2)</t>
+          <t>((17, 1), 2)</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>46.57</v>
+        <v>29.77</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>[((1, 3), 40.6, 0)]</t>
+          <t>[((1, 3), 22.0, 0), ((1, 3), 22.2, 0), ((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0)]</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>[((2, 3), 38.6, 0), ((2, 3), 38.8, 0), ((2, 3), 39.0, 0), ((2, 3), 39.2, 0), ((2, 3), 39.4, 0), ((2, 3), 39.6, 0), ((2, 3), 39.8, 0), ((2, 3), 40.0, 0), ((2, 3), 40.2, 0), ((2, 3), 40.4, 0), ((2, 3), 40.6, 0)]</t>
+          <t>[((2, 3), 13.2, 0), ((2, 3), 13.4, 0), ((2, 3), 13.6, 0), ((2, 3), 13.8, 0), ((2, 3), 14.0, 0), ((2, 3), 14.2, 0), ((2, 3), 14.4, 0), ((2, 3), 14.6, 0), ((2, 3), 14.8, 0), ((2, 3), 15.0, 0)]</t>
         </is>
       </c>
       <c r="E163" t="n">
-        <v>76.67</v>
+        <v>156.7</v>
       </c>
       <c r="F163" t="n">
-        <v>65.66999999999999</v>
+        <v>59.70000000000002</v>
       </c>
       <c r="G163" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 3)</t>
+          <t>((17, 1), 3)</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>52.54</v>
+        <v>35.74</v>
       </c>
       <c r="C164" t="inlineStr"/>
       <c r="D164" t="inlineStr"/>
@@ -4203,7 +4255,7 @@
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 4)</t>
+          <t>((17, 1), 4)</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -4222,7 +4274,7 @@
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>((12, 2), 5)</t>
+          <t>((17, 1), 5)</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
@@ -4241,20 +4293,20 @@
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>((13, 1), 1)</t>
+          <t>((17, 2), 1)</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>24.2</v>
+        <v>43.6</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>[((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0), ((1, 3), 24.0, 0), ((1, 3), 24.2, 0)]</t>
+          <t>[((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0), ((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0)]</t>
         </is>
       </c>
       <c r="D167" t="inlineStr"/>
       <c r="E167" t="n">
-        <v>8.999999999999993</v>
+        <v>9.000000000000014</v>
       </c>
       <c r="F167" t="n">
         <v>119.4</v>
@@ -4266,40 +4318,40 @@
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>((13, 1), 2)</t>
+          <t>((17, 2), 2)</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>30.17</v>
+        <v>49.57</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>[((1, 3), 22.4, 0), ((1, 3), 22.6, 0), ((1, 3), 22.8, 0), ((1, 3), 23.0, 0), ((1, 3), 23.2, 0), ((1, 3), 23.4, 0), ((1, 3), 23.6, 0), ((1, 3), 23.8, 0), ((1, 3), 24.0, 0), ((1, 3), 24.2, 0)]</t>
+          <t>[((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0), ((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0)]</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>[((2, 3), 20.0, 0), ((2, 3), 20.2, 0)]</t>
+          <t>[((2, 3), 33.0, 0), ((2, 3), 33.2, 0), ((2, 3), 33.4, 0), ((2, 3), 33.6, 0), ((2, 3), 33.8, 0), ((2, 3), 34.0, 0), ((2, 3), 34.2, 0), ((2, 3), 34.4, 0), ((2, 3), 34.6, 0), ((2, 3), 34.8, 0)]</t>
         </is>
       </c>
       <c r="E168" t="n">
-        <v>20.14</v>
+        <v>156.7</v>
       </c>
       <c r="F168" t="n">
-        <v>11.94</v>
+        <v>59.69999999999999</v>
       </c>
       <c r="G168" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>((13, 1), 3)</t>
+          <t>((17, 2), 3)</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>36.14</v>
+        <v>55.54</v>
       </c>
       <c r="C169" t="inlineStr"/>
       <c r="D169" t="inlineStr"/>
@@ -4316,7 +4368,7 @@
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>((13, 1), 4)</t>
+          <t>((17, 2), 4)</t>
         </is>
       </c>
       <c r="B170" t="inlineStr"/>
@@ -4335,7 +4387,7 @@
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>((13, 1), 5)</t>
+          <t>((17, 2), 5)</t>
         </is>
       </c>
       <c r="B171" t="inlineStr"/>
@@ -4354,65 +4406,65 @@
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>((13, 2), 1)</t>
+          <t>((18, 1), 1)</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>42.6</v>
+        <v>24</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>[((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0), ((1, 3), 41.6, 0), ((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0)]</t>
+          <t>[((1, 3), 24.0, 0)]</t>
         </is>
       </c>
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="n">
-        <v>9.000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G172" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>((13, 2), 2)</t>
+          <t>((18, 1), 2)</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>48.57</v>
+        <v>29.97</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>[((1, 3), 40.8, 0), ((1, 3), 41.0, 0), ((1, 3), 41.2, 0), ((1, 3), 41.4, 0), ((1, 3), 41.6, 0), ((1, 3), 41.8, 0), ((1, 3), 42.0, 0), ((1, 3), 42.2, 0), ((1, 3), 42.4, 0), ((1, 3), 42.6, 0)]</t>
+          <t>[((1, 3), 24.0, 0)]</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>[((2, 3), 40.8, 0), ((2, 3), 41.0, 0), ((2, 3), 41.2, 0), ((2, 3), 41.4, 0), ((2, 3), 41.6, 0), ((2, 3), 41.8, 0), ((2, 3), 42.0, 0), ((2, 3), 42.2, 0), ((2, 3), 42.4, 0), ((2, 3), 42.6, 0)]</t>
+          <t>[((2, 3), 15.2, 0)]</t>
         </is>
       </c>
       <c r="E173" t="n">
-        <v>68.7</v>
+        <v>14.77</v>
       </c>
       <c r="F173" t="n">
-        <v>59.69999999999999</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G173" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>((13, 2), 3)</t>
+          <t>((18, 1), 3)</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>54.54</v>
+        <v>35.94</v>
       </c>
       <c r="C174" t="inlineStr"/>
       <c r="D174" t="inlineStr"/>
@@ -4429,7 +4481,7 @@
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>((13, 2), 4)</t>
+          <t>((18, 1), 4)</t>
         </is>
       </c>
       <c r="B175" t="inlineStr"/>
@@ -4448,7 +4500,7 @@
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>((13, 2), 5)</t>
+          <t>((18, 1), 5)</t>
         </is>
       </c>
       <c r="B176" t="inlineStr"/>
@@ -4467,65 +4519,65 @@
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>((14, 1), 1)</t>
+          <t>((18, 2), 1)</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>26.2</v>
+        <v>43.8</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>[((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0), ((1, 3), 26.2, 0)]</t>
+          <t>[((1, 3), 43.8, 0)]</t>
         </is>
       </c>
       <c r="D177" t="inlineStr"/>
       <c r="E177" t="n">
-        <v>8.999999999999993</v>
+        <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>119.4</v>
+        <v>11.94</v>
       </c>
       <c r="G177" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>((14, 1), 2)</t>
+          <t>((18, 2), 2)</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>32.17</v>
+        <v>49.77</v>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>[((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0), ((1, 3), 26.2, 0)]</t>
+          <t>[((1, 3), 43.8, 0)]</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>[((2, 3), 20.4, 0), ((2, 3), 20.6, 0), ((2, 3), 20.8, 0), ((2, 3), 21.0, 0), ((2, 3), 21.2, 0), ((2, 3), 21.4, 0), ((2, 3), 21.6, 0), ((2, 3), 21.8, 0), ((2, 3), 22.0, 0), ((2, 3), 22.2, 0)]</t>
+          <t>[((2, 3), 35.0, 0)]</t>
         </is>
       </c>
       <c r="E178" t="n">
-        <v>108.7</v>
+        <v>14.77</v>
       </c>
       <c r="F178" t="n">
-        <v>59.69999999999999</v>
+        <v>5.969999999999999</v>
       </c>
       <c r="G178" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>((14, 1), 3)</t>
+          <t>((18, 2), 3)</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>38.14</v>
+        <v>55.74</v>
       </c>
       <c r="C179" t="inlineStr"/>
       <c r="D179" t="inlineStr"/>
@@ -4542,7 +4594,7 @@
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>((14, 1), 4)</t>
+          <t>((18, 2), 4)</t>
         </is>
       </c>
       <c r="B180" t="inlineStr"/>
@@ -4561,7 +4613,7 @@
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>((14, 1), 5)</t>
+          <t>((18, 2), 5)</t>
         </is>
       </c>
       <c r="B181" t="inlineStr"/>
@@ -4580,20 +4632,20 @@
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>((14, 2), 1)</t>
+          <t>((19, 1), 1)</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>44.6</v>
+        <v>26</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>[((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0), ((1, 3), 43.8, 0), ((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0)]</t>
+          <t>[((1, 3), 24.2, 0), ((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0)]</t>
         </is>
       </c>
       <c r="D182" t="inlineStr"/>
       <c r="E182" t="n">
-        <v>9.000000000000014</v>
+        <v>9</v>
       </c>
       <c r="F182" t="n">
         <v>119.4</v>
@@ -4605,24 +4657,24 @@
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>((14, 2), 2)</t>
+          <t>((19, 1), 2)</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>50.57</v>
+        <v>31.97</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>[((1, 3), 42.8, 0), ((1, 3), 43.0, 0), ((1, 3), 43.2, 0), ((1, 3), 43.4, 0), ((1, 3), 43.6, 0), ((1, 3), 43.8, 0), ((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0)]</t>
+          <t>[((1, 3), 24.2, 0), ((1, 3), 24.4, 0), ((1, 3), 24.6, 0), ((1, 3), 24.8, 0), ((1, 3), 25.0, 0), ((1, 3), 25.2, 0), ((1, 3), 25.4, 0), ((1, 3), 25.6, 0), ((1, 3), 25.8, 0), ((1, 3), 26.0, 0)]</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>[((2, 3), 42.8, 0), ((2, 3), 43.0, 0), ((2, 3), 43.2, 0), ((2, 3), 43.4, 0), ((2, 3), 43.6, 0), ((2, 3), 43.8, 0), ((2, 3), 44.0, 0), ((2, 3), 44.2, 0), ((2, 3), 44.4, 0), ((2, 3), 44.6, 0)]</t>
+          <t>[((2, 3), 15.4, 0), ((2, 3), 15.6, 0), ((2, 3), 15.8, 0), ((2, 3), 16.0, 0), ((2, 3), 16.2, 0), ((2, 3), 16.4, 0), ((2, 3), 16.6, 0), ((2, 3), 16.8, 0), ((2, 3), 17.0, 0), ((2, 3), 17.2, 0)]</t>
         </is>
       </c>
       <c r="E183" t="n">
-        <v>68.7</v>
+        <v>156.7</v>
       </c>
       <c r="F183" t="n">
         <v>59.69999999999999</v>
@@ -4634,11 +4686,11 @@
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>((14, 2), 3)</t>
+          <t>((19, 1), 3)</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>56.54</v>
+        <v>37.94</v>
       </c>
       <c r="C184" t="inlineStr"/>
       <c r="D184" t="inlineStr"/>
@@ -4655,7 +4707,7 @@
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>((14, 2), 4)</t>
+          <t>((19, 1), 4)</t>
         </is>
       </c>
       <c r="B185" t="inlineStr"/>
@@ -4674,7 +4726,7 @@
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>((14, 2), 5)</t>
+          <t>((19, 1), 5)</t>
         </is>
       </c>
       <c r="B186" t="inlineStr"/>
@@ -4690,6 +4742,458 @@
         <v>0</v>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" s="1" t="inlineStr">
+        <is>
+          <t>((19, 2), 1)</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>[((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0), ((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr"/>
+      <c r="E187" t="n">
+        <v>8.999999999999972</v>
+      </c>
+      <c r="F187" t="n">
+        <v>119.4</v>
+      </c>
+      <c r="G187" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="inlineStr">
+        <is>
+          <t>((19, 2), 2)</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>51.77</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>[((1, 3), 44.0, 0), ((1, 3), 44.2, 0), ((1, 3), 44.4, 0), ((1, 3), 44.6, 0), ((1, 3), 44.8, 0), ((1, 3), 45.0, 0), ((1, 3), 45.2, 0), ((1, 3), 45.4, 0), ((1, 3), 45.6, 0), ((1, 3), 45.8, 0)]</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>[((2, 3), 35.2, 0), ((2, 3), 35.4, 0), ((2, 3), 35.6, 0), ((2, 3), 35.8, 0), ((2, 3), 36.0, 0), ((2, 3), 36.2, 0), ((2, 3), 36.4, 0), ((2, 3), 36.6, 0), ((2, 3), 36.8, 0), ((2, 3), 37.0, 0)]</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>156.7</v>
+      </c>
+      <c r="F188" t="n">
+        <v>59.69999999999999</v>
+      </c>
+      <c r="G188" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="inlineStr">
+        <is>
+          <t>((19, 2), 3)</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>57.74</v>
+      </c>
+      <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
+      <c r="E189" t="n">
+        <v>0</v>
+      </c>
+      <c r="F189" t="n">
+        <v>0</v>
+      </c>
+      <c r="G189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="inlineStr">
+        <is>
+          <t>((19, 2), 4)</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr"/>
+      <c r="C190" t="inlineStr"/>
+      <c r="D190" t="inlineStr"/>
+      <c r="E190" t="n">
+        <v>0</v>
+      </c>
+      <c r="F190" t="n">
+        <v>0</v>
+      </c>
+      <c r="G190" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
+        <is>
+          <t>((19, 2), 5)</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr"/>
+      <c r="C191" t="inlineStr"/>
+      <c r="D191" t="inlineStr"/>
+      <c r="E191" t="n">
+        <v>0</v>
+      </c>
+      <c r="F191" t="n">
+        <v>0</v>
+      </c>
+      <c r="G191" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
+        <is>
+          <t>((20, 1), 1)</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>[((1, 3), 26.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr"/>
+      <c r="E192" t="n">
+        <v>0</v>
+      </c>
+      <c r="F192" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="G192" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>((20, 1), 2)</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>32.17</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>[((1, 3), 26.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>[((2, 3), 17.4, 0)]</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>14.77</v>
+      </c>
+      <c r="F193" t="n">
+        <v>5.969999999999999</v>
+      </c>
+      <c r="G193" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
+        <is>
+          <t>((20, 1), 3)</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>38.14</v>
+      </c>
+      <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
+      <c r="E194" t="n">
+        <v>0</v>
+      </c>
+      <c r="F194" t="n">
+        <v>0</v>
+      </c>
+      <c r="G194" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
+        <is>
+          <t>((20, 1), 4)</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
+      <c r="E195" t="n">
+        <v>0</v>
+      </c>
+      <c r="F195" t="n">
+        <v>0</v>
+      </c>
+      <c r="G195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
+        <is>
+          <t>((20, 1), 5)</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr"/>
+      <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
+      <c r="E196" t="n">
+        <v>0</v>
+      </c>
+      <c r="F196" t="n">
+        <v>0</v>
+      </c>
+      <c r="G196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
+        <is>
+          <t>((21, 1), 1)</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>[((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr"/>
+      <c r="E197" t="n">
+        <v>8.999999999999993</v>
+      </c>
+      <c r="F197" t="n">
+        <v>119.4</v>
+      </c>
+      <c r="G197" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
+        <is>
+          <t>((21, 1), 2)</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>34.17</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>[((1, 3), 26.4, 0), ((1, 3), 26.6, 0), ((1, 3), 26.8, 0), ((1, 3), 27.0, 0), ((1, 3), 27.2, 0), ((1, 3), 27.4, 0), ((1, 3), 27.6, 0), ((1, 3), 27.8, 0), ((1, 3), 28.0, 0), ((1, 3), 28.2, 0)]</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>[((2, 3), 17.6, 0), ((2, 3), 17.8, 0), ((2, 3), 18.0, 0), ((2, 3), 18.2, 0), ((2, 3), 18.4, 0), ((2, 3), 18.6, 0), ((2, 3), 18.8, 0), ((2, 3), 19.0, 0), ((2, 3), 19.2, 0), ((2, 3), 19.4, 0)]</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>156.7</v>
+      </c>
+      <c r="F198" t="n">
+        <v>59.69999999999999</v>
+      </c>
+      <c r="G198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
+        <is>
+          <t>((21, 1), 3)</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>40.14</v>
+      </c>
+      <c r="C199" t="inlineStr"/>
+      <c r="D199" t="inlineStr"/>
+      <c r="E199" t="n">
+        <v>0</v>
+      </c>
+      <c r="F199" t="n">
+        <v>0</v>
+      </c>
+      <c r="G199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="inlineStr">
+        <is>
+          <t>((21, 1), 4)</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr"/>
+      <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr"/>
+      <c r="E200" t="n">
+        <v>0</v>
+      </c>
+      <c r="F200" t="n">
+        <v>0</v>
+      </c>
+      <c r="G200" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="inlineStr">
+        <is>
+          <t>((21, 1), 5)</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr"/>
+      <c r="C201" t="inlineStr"/>
+      <c r="D201" t="inlineStr"/>
+      <c r="E201" t="n">
+        <v>0</v>
+      </c>
+      <c r="F201" t="n">
+        <v>0</v>
+      </c>
+      <c r="G201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="inlineStr">
+        <is>
+          <t>((22, 1), 1)</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>[((1, 3), 28.4, 0)]</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr"/>
+      <c r="E202" t="n">
+        <v>0</v>
+      </c>
+      <c r="F202" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="G202" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="inlineStr">
+        <is>
+          <t>((22, 1), 2)</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>34.37</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>[((1, 3), 28.4, 0)]</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>[((2, 3), 19.6, 0)]</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>14.77</v>
+      </c>
+      <c r="F203" t="n">
+        <v>5.970000000000006</v>
+      </c>
+      <c r="G203" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="inlineStr">
+        <is>
+          <t>((22, 1), 3)</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>40.34</v>
+      </c>
+      <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
+      <c r="E204" t="n">
+        <v>0</v>
+      </c>
+      <c r="F204" t="n">
+        <v>0</v>
+      </c>
+      <c r="G204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="inlineStr">
+        <is>
+          <t>((22, 1), 4)</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+      <c r="E205" t="n">
+        <v>0</v>
+      </c>
+      <c r="F205" t="n">
+        <v>0</v>
+      </c>
+      <c r="G205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="inlineStr">
+        <is>
+          <t>((22, 1), 5)</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr"/>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
+      <c r="E206" t="n">
+        <v>0</v>
+      </c>
+      <c r="F206" t="n">
+        <v>0</v>
+      </c>
+      <c r="G206" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>